<commit_message>
Changes to include completed csv data
</commit_message>
<xml_diff>
--- a/app/config/tables/health_facility/forms/health_facility/health_facility.xlsx
+++ b/app/config/tables/health_facility/forms/health_facility/health_facility.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="25180" yWindow="460" windowWidth="26020" windowHeight="26740" tabRatio="500"/>
+    <workbookView xWindow="19720" yWindow="0" windowWidth="31480" windowHeight="28800" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -31,10 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="162">
-  <si>
-    <t>date</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="251">
   <si>
     <t>string</t>
   </si>
@@ -210,18 +207,6 @@
     <t>facility_id</t>
   </si>
   <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>Date Updated</t>
-  </si>
-  <si>
-    <t>date_updated</t>
-  </si>
-  <si>
-    <t>person_in_charge</t>
-  </si>
-  <si>
     <t>facility_type</t>
   </si>
   <si>
@@ -303,9 +288,6 @@
     <t>maternity</t>
   </si>
   <si>
-    <t>ownership</t>
-  </si>
-  <si>
     <t>ownership_types</t>
   </si>
   <si>
@@ -333,21 +315,12 @@
     <t>ngo</t>
   </si>
   <si>
-    <t>faith_based</t>
-  </si>
-  <si>
     <t>other</t>
   </si>
   <si>
-    <t>population</t>
-  </si>
-  <si>
     <t>number</t>
   </si>
   <si>
-    <t>elec_source</t>
-  </si>
-  <si>
     <t>elec_sources</t>
   </si>
   <si>
@@ -372,9 +345,6 @@
     <t>none</t>
   </si>
   <si>
-    <t>grid_availability</t>
-  </si>
-  <si>
     <t>more_than_16</t>
   </si>
   <si>
@@ -432,21 +402,9 @@
     <t>Not Applicable</t>
   </si>
   <si>
-    <t>gas</t>
-  </si>
-  <si>
-    <t>kerosene</t>
-  </si>
-  <si>
-    <t>solar_suitable</t>
-  </si>
-  <si>
     <t>What is the climate of this location?</t>
   </si>
   <si>
-    <t>climate</t>
-  </si>
-  <si>
     <t>climate_types</t>
   </si>
   <si>
@@ -486,15 +444,6 @@
     <t>Choose the ownership</t>
   </si>
   <si>
-    <t>Enter name of the person in charge</t>
-  </si>
-  <si>
-    <t>Enter phone number</t>
-  </si>
-  <si>
-    <t>Enter email</t>
-  </si>
-  <si>
     <t>Enter the facility population</t>
   </si>
   <si>
@@ -510,13 +459,331 @@
     <t>Choose the kerosene availability</t>
   </si>
   <si>
-    <t>Is This a solar suitable site?</t>
-  </si>
-  <si>
     <t>distance_to_supply</t>
   </si>
   <si>
-    <t>phone_number</t>
+    <t>faithbased</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>static</t>
+  </si>
+  <si>
+    <t>Static</t>
+  </si>
+  <si>
+    <t>outreach</t>
+  </si>
+  <si>
+    <t>Outreach</t>
+  </si>
+  <si>
+    <t>Both Static and Outreach</t>
+  </si>
+  <si>
+    <t>storage_types</t>
+  </si>
+  <si>
+    <t>depot</t>
+  </si>
+  <si>
+    <t>Depot</t>
+  </si>
+  <si>
+    <t>delivery</t>
+  </si>
+  <si>
+    <t>Delivery</t>
+  </si>
+  <si>
+    <t>Both Depot and Delivery</t>
+  </si>
+  <si>
+    <t>delivery_types</t>
+  </si>
+  <si>
+    <t>vaccine_modes</t>
+  </si>
+  <si>
+    <t>delivered</t>
+  </si>
+  <si>
+    <t>Delivered</t>
+  </si>
+  <si>
+    <t>collected</t>
+  </si>
+  <si>
+    <t>Collected</t>
+  </si>
+  <si>
+    <t>Both Delivered and Collected</t>
+  </si>
+  <si>
+    <t>facility_name</t>
+  </si>
+  <si>
+    <t>facility_ownership</t>
+  </si>
+  <si>
+    <t>facility_population</t>
+  </si>
+  <si>
+    <t>electricity_source</t>
+  </si>
+  <si>
+    <t>gas_availability</t>
+  </si>
+  <si>
+    <t>kerosene_availability</t>
+  </si>
+  <si>
+    <t>solar_suitable_climate</t>
+  </si>
+  <si>
+    <t>climate_zone</t>
+  </si>
+  <si>
+    <t>admin_region</t>
+  </si>
+  <si>
+    <t>facility_coverage</t>
+  </si>
+  <si>
+    <t>storage_type</t>
+  </si>
+  <si>
+    <t>delivery_type</t>
+  </si>
+  <si>
+    <t>grid_power_availability</t>
+  </si>
+  <si>
+    <t>solar_suitable_site</t>
+  </si>
+  <si>
+    <t>vaccine_supply_interval</t>
+  </si>
+  <si>
+    <t>vaccine_reserve_stock_requirement</t>
+  </si>
+  <si>
+    <t>vaccine_supply_mode</t>
+  </si>
+  <si>
+    <t>contact_name</t>
+  </si>
+  <si>
+    <t>Admin Region</t>
+  </si>
+  <si>
+    <t>regions</t>
+  </si>
+  <si>
+    <t>dowa</t>
+  </si>
+  <si>
+    <t>kasungu</t>
+  </si>
+  <si>
+    <t>nkhotakota</t>
+  </si>
+  <si>
+    <t>ntchisi</t>
+  </si>
+  <si>
+    <t>salima</t>
+  </si>
+  <si>
+    <t>dedza</t>
+  </si>
+  <si>
+    <t>lilongwe</t>
+  </si>
+  <si>
+    <t>mchinji</t>
+  </si>
+  <si>
+    <t>ntcheu</t>
+  </si>
+  <si>
+    <t>chitipa</t>
+  </si>
+  <si>
+    <t>karonga</t>
+  </si>
+  <si>
+    <t>likoma</t>
+  </si>
+  <si>
+    <t>mzimba north</t>
+  </si>
+  <si>
+    <t>mzimba south</t>
+  </si>
+  <si>
+    <t>nkhata bay</t>
+  </si>
+  <si>
+    <t>rumphi</t>
+  </si>
+  <si>
+    <t>balaka</t>
+  </si>
+  <si>
+    <t>machinga</t>
+  </si>
+  <si>
+    <t>mangochi</t>
+  </si>
+  <si>
+    <t>mulanje</t>
+  </si>
+  <si>
+    <t>phalombe</t>
+  </si>
+  <si>
+    <t>zomba</t>
+  </si>
+  <si>
+    <t>blantyre</t>
+  </si>
+  <si>
+    <t>chikwawa</t>
+  </si>
+  <si>
+    <t>chiladzulu</t>
+  </si>
+  <si>
+    <t>mwanza</t>
+  </si>
+  <si>
+    <t>neno</t>
+  </si>
+  <si>
+    <t>nsanje</t>
+  </si>
+  <si>
+    <t>thyolo</t>
+  </si>
+  <si>
+    <t>Dowa</t>
+  </si>
+  <si>
+    <t>Kasungu</t>
+  </si>
+  <si>
+    <t>Nkhotakota</t>
+  </si>
+  <si>
+    <t>Ntchisi</t>
+  </si>
+  <si>
+    <t>Salima</t>
+  </si>
+  <si>
+    <t>Dedza</t>
+  </si>
+  <si>
+    <t>Lilongwe</t>
+  </si>
+  <si>
+    <t>Mchinji</t>
+  </si>
+  <si>
+    <t>Ntcheu</t>
+  </si>
+  <si>
+    <t>Chitipa</t>
+  </si>
+  <si>
+    <t>Karonga</t>
+  </si>
+  <si>
+    <t>Likoma</t>
+  </si>
+  <si>
+    <t>Mzimba North</t>
+  </si>
+  <si>
+    <t>Mzimba South</t>
+  </si>
+  <si>
+    <t>Nkhata Bay</t>
+  </si>
+  <si>
+    <t>Rumphi</t>
+  </si>
+  <si>
+    <t>Balaka</t>
+  </si>
+  <si>
+    <t>Machinga</t>
+  </si>
+  <si>
+    <t>Mangochi</t>
+  </si>
+  <si>
+    <t>Mulanje</t>
+  </si>
+  <si>
+    <t>Phalombe</t>
+  </si>
+  <si>
+    <t>Zomba</t>
+  </si>
+  <si>
+    <t>Blantyre</t>
+  </si>
+  <si>
+    <t>Chikwawa</t>
+  </si>
+  <si>
+    <t>Chiladzulu</t>
+  </si>
+  <si>
+    <t>Mwanza</t>
+  </si>
+  <si>
+    <t>Neno</t>
+  </si>
+  <si>
+    <t>Nsanje</t>
+  </si>
+  <si>
+    <t>Thyolo</t>
+  </si>
+  <si>
+    <t>Percent coverage?</t>
+  </si>
+  <si>
+    <t>Is this a solar suitable site?</t>
+  </si>
+  <si>
+    <t>Is This a solar suitable climate?</t>
+  </si>
+  <si>
+    <t>Storage type?</t>
+  </si>
+  <si>
+    <t>Delivery type?</t>
+  </si>
+  <si>
+    <t>Vaccine Supply Interval?</t>
+  </si>
+  <si>
+    <t>Vaccine Reserve Stock Requirement?</t>
+  </si>
+  <si>
+    <t>Vaccine Supply Mode?</t>
+  </si>
+  <si>
+    <t>Contact Name?</t>
   </si>
 </sst>
 </file>
@@ -874,10 +1141,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -890,31 +1157,31 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="1" t="s">
-        <v>48</v>
+        <v>164</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="E2" s="1" t="b">
         <v>1</v>
@@ -922,13 +1189,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D3" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="E3" t="b">
         <v>1</v>
@@ -936,194 +1203,261 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>59</v>
+      </c>
+      <c r="B4" t="s">
+        <v>183</v>
       </c>
       <c r="C4" t="s">
-        <v>36</v>
+        <v>172</v>
       </c>
       <c r="D4" t="s">
-        <v>148</v>
+        <v>182</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B5" t="s">
-        <v>65</v>
+        <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>63</v>
+        <v>35</v>
       </c>
       <c r="D5" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B6" t="s">
-        <v>91</v>
+        <v>60</v>
       </c>
       <c r="C6" t="s">
-        <v>90</v>
+        <v>58</v>
       </c>
       <c r="D6" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>50</v>
+        <v>59</v>
+      </c>
+      <c r="B7" t="s">
+        <v>85</v>
       </c>
       <c r="C7" t="s">
-        <v>62</v>
+        <v>165</v>
       </c>
       <c r="D7" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>50</v>
+        <v>95</v>
       </c>
       <c r="C8" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="D8" t="s">
-        <v>152</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>95</v>
       </c>
       <c r="C9" t="s">
-        <v>59</v>
+        <v>173</v>
       </c>
       <c r="D9" t="s">
-        <v>153</v>
+        <v>242</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>103</v>
+        <v>59</v>
+      </c>
+      <c r="B10" t="s">
+        <v>96</v>
       </c>
       <c r="C10" t="s">
-        <v>102</v>
+        <v>167</v>
       </c>
       <c r="D10" t="s">
-        <v>154</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B11" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C11" t="s">
-        <v>104</v>
+        <v>176</v>
       </c>
       <c r="D11" t="s">
-        <v>156</v>
+        <v>138</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C12" t="s">
-        <v>109</v>
+        <v>168</v>
       </c>
       <c r="D12" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B13" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="C13" t="s">
-        <v>133</v>
+        <v>169</v>
       </c>
       <c r="D13" t="s">
-        <v>157</v>
+        <v>141</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B14" t="s">
-        <v>122</v>
+        <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>134</v>
+        <v>170</v>
       </c>
       <c r="D14" t="s">
-        <v>158</v>
+        <v>244</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>135</v>
+        <v>177</v>
       </c>
       <c r="D15" t="s">
-        <v>159</v>
+        <v>243</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B16" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="C16" t="s">
-        <v>137</v>
+        <v>171</v>
       </c>
       <c r="D16" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="C17" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="D17" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>0</v>
+        <v>59</v>
+      </c>
+      <c r="B18" t="s">
+        <v>151</v>
       </c>
       <c r="C18" t="s">
-        <v>61</v>
+        <v>174</v>
       </c>
       <c r="D18" t="s">
-        <v>60</v>
-      </c>
-      <c r="E18" t="b">
-        <v>1</v>
+        <v>245</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" t="s">
+        <v>157</v>
+      </c>
+      <c r="C19" t="s">
+        <v>175</v>
+      </c>
+      <c r="D19" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>95</v>
+      </c>
+      <c r="C20" t="s">
+        <v>178</v>
+      </c>
+      <c r="D20" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>95</v>
+      </c>
+      <c r="C21" t="s">
+        <v>179</v>
+      </c>
+      <c r="D21" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22" t="s">
+        <v>158</v>
+      </c>
+      <c r="C22" t="s">
+        <v>180</v>
+      </c>
+      <c r="D22" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" t="s">
+        <v>181</v>
+      </c>
+      <c r="D23" t="s">
+        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -1133,10 +1467,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:C88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1148,409 +1482,860 @@
   <sheetData>
     <row r="1" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C2" t="s">
         <v>16</v>
-      </c>
-      <c r="B2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>145</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B5" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B6" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C6" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B7" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C7" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B8" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C8" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" t="s">
         <v>65</v>
-      </c>
-      <c r="B9" t="s">
-        <v>82</v>
-      </c>
-      <c r="C9" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B10" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C10" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B11" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C11" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B12" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C12" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B13" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C13" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B14" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C14" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B15" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C15" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B16" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C16" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>85</v>
+      </c>
+      <c r="B18" t="s">
         <v>91</v>
       </c>
-      <c r="B18" t="s">
-        <v>97</v>
-      </c>
       <c r="C18" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B19" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C19" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B20" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="C20" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B21" t="s">
-        <v>100</v>
+        <v>143</v>
       </c>
       <c r="C21" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B22" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="C22" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="B24" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="C24" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="B25" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C25" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="B26" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="C26" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="B27" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="C27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="B29" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="C29" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="B30" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="C30" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="B31" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="C31" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="B32" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="C32" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="B33" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="C33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="B35" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="C35" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="B36" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="C36" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="B37" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="C37" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="B38" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C38" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
+        <v>112</v>
+      </c>
+      <c r="B39" t="s">
+        <v>121</v>
+      </c>
+      <c r="C39" t="s">
         <v>122</v>
-      </c>
-      <c r="B39" t="s">
-        <v>131</v>
-      </c>
-      <c r="C39" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="B41" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
       <c r="C41" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="B42" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
       <c r="C42" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="B43" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="C43" t="s">
-        <v>144</v>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>151</v>
+      </c>
+      <c r="B45" t="s">
+        <v>152</v>
+      </c>
+      <c r="C45" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>151</v>
+      </c>
+      <c r="B46" t="s">
+        <v>154</v>
+      </c>
+      <c r="C46" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>151</v>
+      </c>
+      <c r="B47" t="s">
+        <v>102</v>
+      </c>
+      <c r="C47" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>157</v>
+      </c>
+      <c r="B49" t="s">
+        <v>146</v>
+      </c>
+      <c r="C49" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>157</v>
+      </c>
+      <c r="B50" t="s">
+        <v>148</v>
+      </c>
+      <c r="C50" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>157</v>
+      </c>
+      <c r="B51" t="s">
+        <v>102</v>
+      </c>
+      <c r="C51" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>157</v>
+      </c>
+      <c r="B52" t="s">
+        <v>103</v>
+      </c>
+      <c r="C52" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>158</v>
+      </c>
+      <c r="B54" t="s">
+        <v>159</v>
+      </c>
+      <c r="C54" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>158</v>
+      </c>
+      <c r="B55" t="s">
+        <v>161</v>
+      </c>
+      <c r="C55" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>158</v>
+      </c>
+      <c r="B56" t="s">
+        <v>102</v>
+      </c>
+      <c r="C56" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>158</v>
+      </c>
+      <c r="B57" t="s">
+        <v>103</v>
+      </c>
+      <c r="C57" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>158</v>
+      </c>
+      <c r="B58" t="s">
+        <v>119</v>
+      </c>
+      <c r="C58" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>183</v>
+      </c>
+      <c r="B60" t="s">
+        <v>184</v>
+      </c>
+      <c r="C60" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>183</v>
+      </c>
+      <c r="B61" t="s">
+        <v>185</v>
+      </c>
+      <c r="C61" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>183</v>
+      </c>
+      <c r="B62" t="s">
+        <v>186</v>
+      </c>
+      <c r="C62" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>183</v>
+      </c>
+      <c r="B63" t="s">
+        <v>187</v>
+      </c>
+      <c r="C63" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>183</v>
+      </c>
+      <c r="B64" t="s">
+        <v>188</v>
+      </c>
+      <c r="C64" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>183</v>
+      </c>
+      <c r="B65" t="s">
+        <v>189</v>
+      </c>
+      <c r="C65" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>183</v>
+      </c>
+      <c r="B66" t="s">
+        <v>190</v>
+      </c>
+      <c r="C66" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>183</v>
+      </c>
+      <c r="B67" t="s">
+        <v>191</v>
+      </c>
+      <c r="C67" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>183</v>
+      </c>
+      <c r="B68" t="s">
+        <v>192</v>
+      </c>
+      <c r="C68" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>183</v>
+      </c>
+      <c r="B69" t="s">
+        <v>193</v>
+      </c>
+      <c r="C69" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>183</v>
+      </c>
+      <c r="B70" t="s">
+        <v>194</v>
+      </c>
+      <c r="C70" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>183</v>
+      </c>
+      <c r="B71" t="s">
+        <v>195</v>
+      </c>
+      <c r="C71" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>183</v>
+      </c>
+      <c r="B72" t="s">
+        <v>196</v>
+      </c>
+      <c r="C72" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>183</v>
+      </c>
+      <c r="B73" t="s">
+        <v>197</v>
+      </c>
+      <c r="C73" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>183</v>
+      </c>
+      <c r="B74" t="s">
+        <v>198</v>
+      </c>
+      <c r="C74" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>183</v>
+      </c>
+      <c r="B75" t="s">
+        <v>199</v>
+      </c>
+      <c r="C75" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>183</v>
+      </c>
+      <c r="B76" t="s">
+        <v>200</v>
+      </c>
+      <c r="C76" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>183</v>
+      </c>
+      <c r="B77" t="s">
+        <v>201</v>
+      </c>
+      <c r="C77" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>183</v>
+      </c>
+      <c r="B78" t="s">
+        <v>202</v>
+      </c>
+      <c r="C78" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>183</v>
+      </c>
+      <c r="B79" t="s">
+        <v>203</v>
+      </c>
+      <c r="C79" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>183</v>
+      </c>
+      <c r="B80" t="s">
+        <v>204</v>
+      </c>
+      <c r="C80" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>183</v>
+      </c>
+      <c r="B81" t="s">
+        <v>205</v>
+      </c>
+      <c r="C81" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>183</v>
+      </c>
+      <c r="B82" t="s">
+        <v>206</v>
+      </c>
+      <c r="C82" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>183</v>
+      </c>
+      <c r="B83" t="s">
+        <v>207</v>
+      </c>
+      <c r="C83" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>183</v>
+      </c>
+      <c r="B84" t="s">
+        <v>208</v>
+      </c>
+      <c r="C84" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>183</v>
+      </c>
+      <c r="B85" t="s">
+        <v>209</v>
+      </c>
+      <c r="C85" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>183</v>
+      </c>
+      <c r="B86" t="s">
+        <v>210</v>
+      </c>
+      <c r="C86" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>183</v>
+      </c>
+      <c r="B87" t="s">
+        <v>211</v>
+      </c>
+      <c r="C87" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>183</v>
+      </c>
+      <c r="B88" t="s">
+        <v>212</v>
+      </c>
+      <c r="C88" t="s">
+        <v>241</v>
       </c>
     </row>
   </sheetData>
@@ -1579,48 +2364,48 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" t="s">
         <v>55</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" t="s">
         <v>44</v>
       </c>
-      <c r="C2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>45</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" s="6" t="s">
         <v>46</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1643,42 +2428,42 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>10</v>
-      </c>
-      <c r="C1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="2" t="b">
         <v>1</v>
@@ -1686,10 +2471,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1709,138 +2494,138 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
         <v>19</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>20</v>
       </c>
-      <c r="C1" t="s">
-        <v>21</v>
-      </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
         <v>22</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>23</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
         <v>24</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
         <v>22</v>
       </c>
-      <c r="B3" t="s">
-        <v>23</v>
-      </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
         <v>22</v>
       </c>
-      <c r="B4" t="s">
-        <v>23</v>
-      </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
         <v>22</v>
       </c>
-      <c r="B5" t="s">
-        <v>23</v>
-      </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
         <v>29</v>
       </c>
-      <c r="B6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
         <v>30</v>
-      </c>
-      <c r="D6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
         <v>32</v>
-      </c>
-      <c r="D7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E7" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
         <v>34</v>
-      </c>
-      <c r="D8" t="s">
-        <v>1</v>
-      </c>
-      <c r="E8" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented search feature, fixed survey, added refrigerator model photos
</commit_message>
<xml_diff>
--- a/app/config/tables/health_facility/forms/health_facility/health_facility.xlsx
+++ b/app/config/tables/health_facility/forms/health_facility/health_facility.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="19720" yWindow="0" windowWidth="31480" windowHeight="28800" tabRatio="500"/>
+    <workbookView xWindow="13300" yWindow="460" windowWidth="51200" windowHeight="26740" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="250">
   <si>
     <t>string</t>
   </si>
@@ -174,9 +174,6 @@
     <t>'_id&gt;='+opendatakit.encodeURIValue(0)</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
     <t>instance_name</t>
   </si>
   <si>
@@ -765,9 +762,6 @@
     <t>Is this a solar suitable site?</t>
   </si>
   <si>
-    <t>Is This a solar suitable climate?</t>
-  </si>
-  <si>
     <t>Storage type?</t>
   </si>
   <si>
@@ -784,6 +778,9 @@
   </si>
   <si>
     <t>Contact Name?</t>
+  </si>
+  <si>
+    <t>Is this a solar suitable climate?</t>
   </si>
 </sst>
 </file>
@@ -1143,8 +1140,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1169,19 +1166,19 @@
         <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E2" s="1" t="b">
         <v>1</v>
@@ -1189,13 +1186,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E3" t="b">
         <v>1</v>
@@ -1203,16 +1200,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -1223,241 +1220,241 @@
         <v>35</v>
       </c>
       <c r="D5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" t="s">
         <v>59</v>
       </c>
-      <c r="B6" t="s">
-        <v>60</v>
-      </c>
       <c r="C6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D9" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C10" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C11" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C12" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C13" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B14" t="s">
         <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D14" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B15" t="s">
         <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D15" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C16" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C17" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B18" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C18" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D18" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B19" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C19" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D19" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C20" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D20" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C21" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D21" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B22" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C22" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D22" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C23" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D23" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
   </sheetData>
@@ -1496,7 +1493,7 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C2" t="s">
         <v>16</v>
@@ -1507,7 +1504,7 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C3" t="s">
         <v>17</v>
@@ -1515,230 +1512,230 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C5" t="s">
         <v>60</v>
-      </c>
-      <c r="B5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C5" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>84</v>
+      </c>
+      <c r="B18" t="s">
+        <v>90</v>
+      </c>
+      <c r="C18" t="s">
         <v>85</v>
-      </c>
-      <c r="B18" t="s">
-        <v>91</v>
-      </c>
-      <c r="C18" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B21" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B22" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C22" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>95</v>
+      </c>
+      <c r="B24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C24" t="s">
         <v>96</v>
-      </c>
-      <c r="B24" t="s">
-        <v>100</v>
-      </c>
-      <c r="C24" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B26" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B27" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C27" t="s">
         <v>30</v>
@@ -1746,54 +1743,54 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B29" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C29" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B30" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B31" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C31" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B32" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C32" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C33" t="s">
         <v>30</v>
@@ -1801,164 +1798,164 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
+        <v>111</v>
+      </c>
+      <c r="B35" t="s">
         <v>112</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
         <v>113</v>
-      </c>
-      <c r="C35" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B36" t="s">
+        <v>114</v>
+      </c>
+      <c r="C36" t="s">
         <v>115</v>
-      </c>
-      <c r="C36" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B37" t="s">
+        <v>116</v>
+      </c>
+      <c r="C37" t="s">
         <v>117</v>
-      </c>
-      <c r="C37" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B38" t="s">
+        <v>118</v>
+      </c>
+      <c r="C38" t="s">
         <v>119</v>
-      </c>
-      <c r="C38" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B39" t="s">
+        <v>120</v>
+      </c>
+      <c r="C39" t="s">
         <v>121</v>
-      </c>
-      <c r="C39" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
+        <v>123</v>
+      </c>
+      <c r="B41" t="s">
         <v>124</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C41" t="s">
         <v>125</v>
-      </c>
-      <c r="C41" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B42" t="s">
+        <v>126</v>
+      </c>
+      <c r="C42" t="s">
         <v>127</v>
-      </c>
-      <c r="C42" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B43" t="s">
+        <v>128</v>
+      </c>
+      <c r="C43" t="s">
         <v>129</v>
-      </c>
-      <c r="C43" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
+        <v>150</v>
+      </c>
+      <c r="B45" t="s">
         <v>151</v>
       </c>
-      <c r="B45" t="s">
+      <c r="C45" t="s">
         <v>152</v>
-      </c>
-      <c r="C45" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B46" t="s">
+        <v>153</v>
+      </c>
+      <c r="C46" t="s">
         <v>154</v>
-      </c>
-      <c r="C46" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B47" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C47" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B49" t="s">
+        <v>145</v>
+      </c>
+      <c r="C49" t="s">
         <v>146</v>
-      </c>
-      <c r="C49" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B50" t="s">
+        <v>147</v>
+      </c>
+      <c r="C50" t="s">
         <v>148</v>
-      </c>
-      <c r="C50" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B51" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C51" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B52" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C52" t="s">
         <v>30</v>
@@ -1966,43 +1963,43 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
+        <v>157</v>
+      </c>
+      <c r="B54" t="s">
         <v>158</v>
       </c>
-      <c r="B54" t="s">
+      <c r="C54" t="s">
         <v>159</v>
-      </c>
-      <c r="C54" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B55" t="s">
+        <v>160</v>
+      </c>
+      <c r="C55" t="s">
         <v>161</v>
-      </c>
-      <c r="C55" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B56" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C56" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B57" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C57" t="s">
         <v>30</v>
@@ -2010,332 +2007,332 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B58" t="s">
+        <v>118</v>
+      </c>
+      <c r="C58" t="s">
         <v>119</v>
-      </c>
-      <c r="C58" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
+        <v>182</v>
+      </c>
+      <c r="B60" t="s">
         <v>183</v>
       </c>
-      <c r="B60" t="s">
-        <v>184</v>
-      </c>
       <c r="C60" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B61" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C61" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B62" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C62" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B63" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C63" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B64" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C64" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B65" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C65" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B66" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C66" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B67" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C67" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B68" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C68" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B69" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C69" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B70" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C70" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B71" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C71" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B72" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C72" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B73" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C73" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B74" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C74" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B75" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C75" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B76" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C76" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B77" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C77" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B78" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C78" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B79" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C79" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B80" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C80" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B81" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C81" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B82" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C82" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B83" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C83" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B84" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C84" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B85" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C85" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B86" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C86" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B87" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C87" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B88" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C88" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
   </sheetData>
@@ -2387,16 +2384,16 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B2" t="s">
         <v>43</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E2" t="s">
         <v>44</v>
@@ -2417,8 +2414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2442,7 +2439,7 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -2450,7 +2447,7 @@
         <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -2458,7 +2455,7 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -2471,10 +2468,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -2540,7 +2537,7 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -2557,7 +2554,7 @@
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -2574,7 +2571,7 @@
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Fix some translations for survey
</commit_message>
<xml_diff>
--- a/app/config/tables/health_facility/forms/health_facility/health_facility.xlsx
+++ b/app/config/tables/health_facility/forms/health_facility/health_facility.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="223">
   <si>
     <t xml:space="preserve">clause</t>
   </si>
@@ -41,238 +41,241 @@
     <t xml:space="preserve">name</t>
   </si>
   <si>
+    <t xml:space="preserve">display.prompt.text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">choice_filter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">required</t>
+  </si>
+  <si>
+    <t xml:space="preserve">begin screen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">facility_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enter health facility name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">facility_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enter health facility ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">end screen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">geopoint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Capture location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select_one_dropdown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">regionLevel1_csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">regionLevel1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Level 1 of admin region</t>
+  </si>
+  <si>
+    <t xml:space="preserve">regionLevel2_csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">regionLevel2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Level 2 of admin region</t>
+  </si>
+  <si>
+    <t xml:space="preserve">choice_item.regionLevel1 === data('regionLevel1')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">regionLevel3_csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">admin_region</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Admin Region</t>
+  </si>
+  <si>
+    <t xml:space="preserve">choice_item.regionLevel2 === data('regionLevel2')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select_one</t>
+  </si>
+  <si>
+    <t xml:space="preserve">facility_types</t>
+  </si>
+  <si>
+    <t xml:space="preserve">facility_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Choose the facility type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ownership_types</t>
+  </si>
+  <si>
+    <t xml:space="preserve">facility_ownership</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Choose the ownership</t>
+  </si>
+  <si>
+    <t xml:space="preserve">number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">facility_population</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enter the facility population</t>
+  </si>
+  <si>
+    <t xml:space="preserve">facility_coverage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percent coverage?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">elec_sources</t>
+  </si>
+  <si>
+    <t xml:space="preserve">electricity_source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Choose the electricity source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if</t>
+  </si>
+  <si>
+    <t xml:space="preserve">selected(data('electricity_source'), 'grid')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grid_power_availability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Choose the grid availability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">end if</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fuel_availability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gas_availability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Choose the gas availability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kerosene_availability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Choose the kerosene availability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes_no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">solar_suitable_climate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is this a solar suitable climate?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">solar_suitable_site</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is this a solar suitable site?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">climate_types</t>
+  </si>
+  <si>
+    <t xml:space="preserve">climate_zone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is the climate of this location?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">distance_to_supply</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is the distance to the nearest supply point?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">storage_types</t>
+  </si>
+  <si>
+    <t xml:space="preserve">storage_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Storage type?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">delivery_types</t>
+  </si>
+  <si>
+    <t xml:space="preserve">delivery_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delivery type?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vaccine_supply_interval</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vaccine Supply Interval?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vaccine_reserve_stock_requirement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vaccine Reserve Stock Requirement?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vaccine_modes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vaccine_supply_mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vaccine Supply Mode?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contact_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact Name?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">choice_list_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data_value</t>
+  </si>
+  <si>
     <t xml:space="preserve">display.text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">choice_filter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">required</t>
-  </si>
-  <si>
-    <t xml:space="preserve">begin screen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">facility_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enter health facility name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">facility_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enter health facility ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">end screen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">geopoint</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Location</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Capture location</t>
-  </si>
-  <si>
-    <t xml:space="preserve">select_one_dropdown</t>
-  </si>
-  <si>
-    <t xml:space="preserve">regionLevel1_csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">regionLevel1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Level 1 of admin region</t>
-  </si>
-  <si>
-    <t xml:space="preserve">regionLevel2_csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">regionLevel2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Level 2 of admin region</t>
-  </si>
-  <si>
-    <t xml:space="preserve">choice_item.regionLevel1 === data('regionLevel1')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">regionLevel3_csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">admin_region</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Admin Region</t>
-  </si>
-  <si>
-    <t xml:space="preserve">choice_item.regionLevel2 === data('regionLevel2')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">select_one</t>
-  </si>
-  <si>
-    <t xml:space="preserve">facility_types</t>
-  </si>
-  <si>
-    <t xml:space="preserve">facility_type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Choose the facility type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ownership_types</t>
-  </si>
-  <si>
-    <t xml:space="preserve">facility_ownership</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Choose the ownership</t>
-  </si>
-  <si>
-    <t xml:space="preserve">number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">facility_population</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enter the facility population</t>
-  </si>
-  <si>
-    <t xml:space="preserve">facility_coverage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percent coverage?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">elec_sources</t>
-  </si>
-  <si>
-    <t xml:space="preserve">electricity_source</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Choose the electricity source</t>
-  </si>
-  <si>
-    <t xml:space="preserve">if</t>
-  </si>
-  <si>
-    <t xml:space="preserve">selected(data('electricity_source'), 'grid')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">grid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">grid_power_availability</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Choose the grid availability</t>
-  </si>
-  <si>
-    <t xml:space="preserve">end if</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fuel_availability</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gas_availability</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Choose the gas availability</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kerosene_availability</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Choose the kerosene availability</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yes_no</t>
-  </si>
-  <si>
-    <t xml:space="preserve">solar_suitable_climate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Is this a solar suitable climate?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">solar_suitable_site</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Is this a solar suitable site?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">climate_types</t>
-  </si>
-  <si>
-    <t xml:space="preserve">climate_zone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">What is the climate of this location?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">distance_to_supply</t>
-  </si>
-  <si>
-    <t xml:space="preserve">What is the distance to the nearest supply point?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">storage_types</t>
-  </si>
-  <si>
-    <t xml:space="preserve">storage_type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Storage type?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">delivery_types</t>
-  </si>
-  <si>
-    <t xml:space="preserve">delivery_type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Delivery type?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vaccine_supply_interval</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vaccine Supply Interval?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vaccine_reserve_stock_requirement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vaccine Reserve Stock Requirement?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vaccine_modes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vaccine_supply_mode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vaccine Supply Mode?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">contact_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contact Name?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">choice_list_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">data_value</t>
   </si>
   <si>
     <t xml:space="preserve">yes</t>
@@ -898,8 +901,8 @@
   </sheetPr>
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G10" activeCellId="1" sqref="B8 G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -913,7 +916,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="10.49"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -1372,7 +1375,7 @@
   <dimension ref="A1:C58"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B83" activeCellId="0" sqref="B83"/>
+      <selection pane="topLeft" activeCell="B83" activeCellId="1" sqref="B8 B83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1391,7 +1394,7 @@
         <v>82</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1399,10 +1402,10 @@
         <v>56</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1410,10 +1413,10 @@
         <v>56</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1421,10 +1424,10 @@
         <v>31</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1432,10 +1435,10 @@
         <v>31</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1443,10 +1446,10 @@
         <v>31</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1454,10 +1457,10 @@
         <v>31</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1465,10 +1468,10 @@
         <v>31</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1476,10 +1479,10 @@
         <v>31</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1487,10 +1490,10 @@
         <v>31</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1498,10 +1501,10 @@
         <v>31</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1509,10 +1512,10 @@
         <v>31</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1520,10 +1523,10 @@
         <v>31</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1531,10 +1534,10 @@
         <v>31</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1542,10 +1545,10 @@
         <v>31</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1553,10 +1556,10 @@
         <v>34</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1564,10 +1567,10 @@
         <v>34</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1575,10 +1578,10 @@
         <v>34</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1586,10 +1589,10 @@
         <v>34</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1597,10 +1600,10 @@
         <v>34</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1611,7 +1614,7 @@
         <v>47</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1619,10 +1622,10 @@
         <v>42</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1630,10 +1633,10 @@
         <v>42</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1641,10 +1644,10 @@
         <v>42</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1652,10 +1655,10 @@
         <v>47</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1663,10 +1666,10 @@
         <v>47</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1674,10 +1677,10 @@
         <v>47</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1685,10 +1688,10 @@
         <v>47</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1696,10 +1699,10 @@
         <v>47</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1707,10 +1710,10 @@
         <v>51</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1718,10 +1721,10 @@
         <v>51</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1729,10 +1732,10 @@
         <v>51</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1740,10 +1743,10 @@
         <v>51</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1751,10 +1754,10 @@
         <v>51</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1762,10 +1765,10 @@
         <v>61</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1773,10 +1776,10 @@
         <v>61</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1784,10 +1787,10 @@
         <v>61</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1795,10 +1798,10 @@
         <v>66</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1806,10 +1809,10 @@
         <v>66</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1817,10 +1820,10 @@
         <v>66</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1828,10 +1831,10 @@
         <v>69</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1839,10 +1842,10 @@
         <v>69</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1850,10 +1853,10 @@
         <v>69</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1861,10 +1864,10 @@
         <v>69</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1872,10 +1875,10 @@
         <v>76</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1883,10 +1886,10 @@
         <v>76</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1894,10 +1897,10 @@
         <v>76</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1905,10 +1908,10 @@
         <v>76</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1916,10 +1919,10 @@
         <v>76</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -1940,8 +1943,8 @@
   </sheetPr>
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J8" activeCellId="1" sqref="B8 J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1962,66 +1965,66 @@
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="45.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2029,19 +2032,19 @@
         <v>19</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="J3" s="0" t="s">
         <v>185</v>
       </c>
-      <c r="H3" s="0" t="s">
-        <v>186</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="J3" s="0" t="s">
-        <v>184</v>
-      </c>
       <c r="K3" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="64.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2049,19 +2052,19 @@
         <v>22</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J4" s="0" t="s">
         <v>185</v>
       </c>
-      <c r="H4" s="0" t="s">
-        <v>186</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="J4" s="0" t="s">
-        <v>184</v>
-      </c>
       <c r="K4" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="62" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2069,19 +2072,19 @@
         <v>26</v>
       </c>
       <c r="B5" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="J5" s="0" t="s">
         <v>185</v>
       </c>
-      <c r="H5" s="0" t="s">
-        <v>189</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="J5" s="0" t="s">
-        <v>184</v>
-      </c>
       <c r="K5" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -2102,8 +2105,8 @@
   </sheetPr>
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2114,42 +2117,42 @@
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B6" s="2" t="n">
         <f aca="false">TRUE()</f>
@@ -2158,7 +2161,7 @@
     </row>
     <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>10</v>
@@ -2166,10 +2169,10 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B8" s="7" t="n">
-        <v>20170713</v>
+        <v>20170714</v>
       </c>
     </row>
   </sheetData>
@@ -2190,8 +2193,8 @@
   </sheetPr>
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E4" activeCellId="1" sqref="B8 E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2201,138 +2204,138 @@
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D1" s="0" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix a choice value that didn't match up with the value in the csv files and was causing translation errors
</commit_message>
<xml_diff>
--- a/app/config/tables/health_facility/forms/health_facility/health_facility.xlsx
+++ b/app/config/tables/health_facility/forms/health_facility/health_facility.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
@@ -443,10 +443,10 @@
     <t xml:space="preserve">Hospital de comunidad</t>
   </si>
   <si>
-    <t xml:space="preserve">health_centre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Health centre</t>
+    <t xml:space="preserve">health_center</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Health center</t>
   </si>
   <si>
     <t xml:space="preserve">Centro de salud</t>
@@ -1129,8 +1129,8 @@
   </sheetPr>
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G38" activeCellId="0" sqref="G38"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1679,8 +1679,8 @@
   </sheetPr>
   <dimension ref="A1:D58"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E58" activeCellId="0" sqref="E58"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2558,7 +2558,7 @@
   </sheetPr>
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Spanish translations for names
</commit_message>
<xml_diff>
--- a/app/config/tables/health_facility/forms/health_facility/health_facility.xlsx
+++ b/app/config/tables/health_facility/forms/health_facility/health_facility.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="323">
   <si>
     <t xml:space="preserve">clause</t>
   </si>
@@ -41,10 +41,16 @@
     <t xml:space="preserve">name</t>
   </si>
   <si>
+    <t xml:space="preserve">display.title.text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">display.title.text.es</t>
+  </si>
+  <si>
     <t xml:space="preserve">display.prompt.text</t>
   </si>
   <si>
-    <t xml:space="preserve">display.prompt.text.spanish</t>
+    <t xml:space="preserve">display.prompt.text.es</t>
   </si>
   <si>
     <t xml:space="preserve">choice_filter</t>
@@ -62,21 +68,27 @@
     <t xml:space="preserve">facility_name</t>
   </si>
   <si>
+    <t xml:space="preserve">Facility Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nombre de Facilidad</t>
+  </si>
+  <si>
     <t xml:space="preserve">Enter health facility name</t>
   </si>
   <si>
-    <t xml:space="preserve">Nombre de Facilidad</t>
-  </si>
-  <si>
     <t xml:space="preserve">facility_id</t>
   </si>
   <si>
+    <t xml:space="preserve">Facility ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID de Facilidad</t>
+  </si>
+  <si>
     <t xml:space="preserve">Enter health facility ID</t>
   </si>
   <si>
-    <t xml:space="preserve">ID de Facilidad</t>
-  </si>
-  <si>
     <t xml:space="preserve">end screen</t>
   </si>
   <si>
@@ -86,12 +98,12 @@
     <t xml:space="preserve">Location</t>
   </si>
   <si>
+    <t xml:space="preserve">Ubicación</t>
+  </si>
+  <si>
     <t xml:space="preserve">Capture location</t>
   </si>
   <si>
-    <t xml:space="preserve">Ubicación</t>
-  </si>
-  <si>
     <t xml:space="preserve">select_one_dropdown</t>
   </si>
   <si>
@@ -101,24 +113,30 @@
     <t xml:space="preserve">regionLevel1</t>
   </si>
   <si>
+    <t xml:space="preserve">Region Level 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nievel uno de region administrativo</t>
+  </si>
+  <si>
     <t xml:space="preserve">Level 1 of admin region</t>
   </si>
   <si>
-    <t xml:space="preserve">Nievel uno de region administrativo</t>
-  </si>
-  <si>
     <t xml:space="preserve">regionLevel2_csv</t>
   </si>
   <si>
     <t xml:space="preserve">regionLevel2</t>
   </si>
   <si>
+    <t xml:space="preserve">Region Level 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nievel dos de region administrativo</t>
+  </si>
+  <si>
     <t xml:space="preserve">Level 2 of admin region</t>
   </si>
   <si>
-    <t xml:space="preserve">Nievel dos de region administrativo</t>
-  </si>
-  <si>
     <t xml:space="preserve">choice_item.regionLevel1 === data('regionLevel1')</t>
   </si>
   <si>
@@ -146,57 +164,72 @@
     <t xml:space="preserve">facility_type</t>
   </si>
   <si>
+    <t xml:space="preserve">Facility Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tipo de facilidad</t>
+  </si>
+  <si>
     <t xml:space="preserve">Choose the facility type</t>
   </si>
   <si>
-    <t xml:space="preserve">Tipo de facilidad</t>
-  </si>
-  <si>
     <t xml:space="preserve">ownership_types</t>
   </si>
   <si>
     <t xml:space="preserve">facility_ownership</t>
   </si>
   <si>
+    <t xml:space="preserve">Facility Ownership</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tipo de propriedad</t>
+  </si>
+  <si>
     <t xml:space="preserve">Choose the ownership</t>
   </si>
   <si>
-    <t xml:space="preserve">Tipo de propriedad</t>
-  </si>
-  <si>
     <t xml:space="preserve">number</t>
   </si>
   <si>
     <t xml:space="preserve">facility_population</t>
   </si>
   <si>
+    <t xml:space="preserve">Facility Population</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Población de facilidad</t>
+  </si>
+  <si>
     <t xml:space="preserve">Enter the facility population</t>
   </si>
   <si>
-    <t xml:space="preserve">Población de facilidad</t>
-  </si>
-  <si>
     <t xml:space="preserve">facility_coverage</t>
   </si>
   <si>
+    <t xml:space="preserve">Facility Coverage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cobertura (porcentaje)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Percent coverage?</t>
   </si>
   <si>
-    <t xml:space="preserve">Cobertura (porcentaje)</t>
-  </si>
-  <si>
     <t xml:space="preserve">elec_sources</t>
   </si>
   <si>
     <t xml:space="preserve">electricity_source</t>
   </si>
   <si>
+    <t xml:space="preserve">Electricity Source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fuente de energía</t>
+  </si>
+  <si>
     <t xml:space="preserve">Choose the electricity source</t>
   </si>
   <si>
-    <t xml:space="preserve">Fuente de energía</t>
-  </si>
-  <si>
     <t xml:space="preserve">if</t>
   </si>
   <si>
@@ -209,12 +242,15 @@
     <t xml:space="preserve">grid_power_availability</t>
   </si>
   <si>
+    <t xml:space="preserve">Grid Availability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Disponibilidad del red de energía</t>
+  </si>
+  <si>
     <t xml:space="preserve">Choose the grid availability</t>
   </si>
   <si>
-    <t xml:space="preserve">Disponibilidad del red de energía</t>
-  </si>
-  <si>
     <t xml:space="preserve">end if</t>
   </si>
   <si>
@@ -224,27 +260,39 @@
     <t xml:space="preserve">gas_availability</t>
   </si>
   <si>
+    <t xml:space="preserve">Gas Availability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Disponibilidad de combustible</t>
+  </si>
+  <si>
     <t xml:space="preserve">Choose the gas availability</t>
   </si>
   <si>
-    <t xml:space="preserve">Disponibilidad de combustible</t>
-  </si>
-  <si>
     <t xml:space="preserve">kerosene_availability</t>
   </si>
   <si>
+    <t xml:space="preserve">Kerosene Availability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Disponibilidad de queroseno</t>
+  </si>
+  <si>
     <t xml:space="preserve">Choose the kerosene availability</t>
   </si>
   <si>
-    <t xml:space="preserve">Disponibilidad de queroseno</t>
-  </si>
-  <si>
     <t xml:space="preserve">yes_no</t>
   </si>
   <si>
     <t xml:space="preserve">solar_suitable_climate</t>
   </si>
   <si>
+    <t xml:space="preserve">Solar Suitable Climate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clima adecuedo por energía solár</t>
+  </si>
+  <si>
     <t xml:space="preserve">Is this a solar suitable climate?</t>
   </si>
   <si>
@@ -254,6 +302,12 @@
     <t xml:space="preserve">solar_suitable_site</t>
   </si>
   <si>
+    <t xml:space="preserve">Solar Suitable Site</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Facilidad adecuedo por energía solar</t>
+  </si>
+  <si>
     <t xml:space="preserve">Is this a solar suitable site?</t>
   </si>
   <si>
@@ -266,84 +320,108 @@
     <t xml:space="preserve">climate_zone</t>
   </si>
   <si>
+    <t xml:space="preserve">Climate Zone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clima de ubicación</t>
+  </si>
+  <si>
     <t xml:space="preserve">What is the climate of this location?</t>
   </si>
   <si>
-    <t xml:space="preserve">Clima de ubicación</t>
-  </si>
-  <si>
     <t xml:space="preserve">distance_to_supply</t>
   </si>
   <si>
+    <t xml:space="preserve">Distance to the Closest Supply Point</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Distancia al más proximo punto de reabastecimiento</t>
+  </si>
+  <si>
     <t xml:space="preserve">What is the distance to the nearest supply point?</t>
   </si>
   <si>
-    <t xml:space="preserve">Distancia al más proximo punto de reabastecimiento</t>
-  </si>
-  <si>
     <t xml:space="preserve">storage_types</t>
   </si>
   <si>
     <t xml:space="preserve">storage_type</t>
   </si>
   <si>
+    <t xml:space="preserve">Storage Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tipo de almacenamiento</t>
+  </si>
+  <si>
     <t xml:space="preserve">Storage type?</t>
   </si>
   <si>
-    <t xml:space="preserve">Tipo de almacenamiento</t>
-  </si>
-  <si>
     <t xml:space="preserve">delivery_types</t>
   </si>
   <si>
     <t xml:space="preserve">delivery_type</t>
   </si>
   <si>
+    <t xml:space="preserve">Delivery Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tipo de envío</t>
+  </si>
+  <si>
     <t xml:space="preserve">Delivery type?</t>
   </si>
   <si>
-    <t xml:space="preserve">Tipo de envío</t>
-  </si>
-  <si>
     <t xml:space="preserve">vaccine_supply_interval</t>
   </si>
   <si>
+    <t xml:space="preserve">Supply Interval</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intervalo de reabastecimiento</t>
+  </si>
+  <si>
     <t xml:space="preserve">Vaccine Supply Interval?</t>
   </si>
   <si>
-    <t xml:space="preserve">Intervalo de reabastecimiento</t>
-  </si>
-  <si>
     <t xml:space="preserve">vaccine_reserve_stock_requirement</t>
   </si>
   <si>
+    <t xml:space="preserve">Minimum Reserve Requirement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tamaño Minimo de Reserva</t>
+  </si>
+  <si>
     <t xml:space="preserve">Vaccine Reserve Stock Requirement?</t>
   </si>
   <si>
-    <t xml:space="preserve">Tamaño Minimo de Reserva</t>
-  </si>
-  <si>
     <t xml:space="preserve">vaccine_modes</t>
   </si>
   <si>
     <t xml:space="preserve">vaccine_supply_mode</t>
   </si>
   <si>
+    <t xml:space="preserve">Supply Mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modo de recibir vacunas</t>
+  </si>
+  <si>
     <t xml:space="preserve">Vaccine Supply Mode?</t>
   </si>
   <si>
-    <t xml:space="preserve">Modo de recibir vacunas</t>
-  </si>
-  <si>
     <t xml:space="preserve">contact_name</t>
   </si>
   <si>
+    <t xml:space="preserve">Contact Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nombre del contacto</t>
+  </si>
+  <si>
     <t xml:space="preserve">Contact Name?</t>
   </si>
   <si>
-    <t xml:space="preserve">Nombre del contacto</t>
-  </si>
-  <si>
     <t xml:space="preserve">choice_list_name</t>
   </si>
   <si>
@@ -353,7 +431,7 @@
     <t xml:space="preserve">display.text</t>
   </si>
   <si>
-    <t xml:space="preserve">display.text.spanish</t>
+    <t xml:space="preserve">display.text.es</t>
   </si>
   <si>
     <t xml:space="preserve">yes</t>
@@ -809,16 +887,10 @@
     <t xml:space="preserve">value</t>
   </si>
   <si>
-    <t xml:space="preserve">display.title.text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">display.title.text.spanish</t>
-  </si>
-  <si>
     <t xml:space="preserve">display.locale.text</t>
   </si>
   <si>
-    <t xml:space="preserve">display.locale.text.spanish</t>
+    <t xml:space="preserve">display.locale.text.es</t>
   </si>
   <si>
     <t xml:space="preserve">form_id</t>
@@ -857,7 +929,7 @@
     <t xml:space="preserve">Inglés</t>
   </si>
   <si>
-    <t xml:space="preserve">spanish</t>
+    <t xml:space="preserve">es</t>
   </si>
   <si>
     <t xml:space="preserve">Spanish</t>
@@ -1127,10 +1199,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I41"/>
+  <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1140,9 +1212,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="26.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="47.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="10.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="0" width="26.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="47.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="10.49"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1173,10 +1245,16 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="2"/>
@@ -1185,480 +1263,626 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" s="0" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="0" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" s="0" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="0" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>26</v>
+        <v>30</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="I8" s="0" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>31</v>
+        <v>36</v>
+      </c>
+      <c r="I9" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="J9" s="0" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>36</v>
+        <v>40</v>
+      </c>
+      <c r="I10" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="J10" s="0" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="0" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>41</v>
+        <v>47</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="I13" s="0" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="0" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>45</v>
+        <v>52</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="I14" s="0" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="0" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>49</v>
+        <v>57</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="I15" s="0" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="0" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>52</v>
+        <v>61</v>
+      </c>
+      <c r="H16" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="I16" s="0" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C19" s="0" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>56</v>
+        <v>66</v>
+      </c>
+      <c r="H19" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="I19" s="0" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="0" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>62</v>
+        <v>73</v>
+      </c>
+      <c r="H21" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="I21" s="0" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="0" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>67</v>
+        <v>79</v>
+      </c>
+      <c r="H23" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="I23" s="0" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C24" s="0" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>70</v>
+        <v>83</v>
+      </c>
+      <c r="H24" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="I24" s="0" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="0" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>74</v>
+        <v>88</v>
+      </c>
+      <c r="H27" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="I27" s="0" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C28" s="0" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>77</v>
+        <v>93</v>
+      </c>
+      <c r="H28" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="I28" s="0" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C29" s="0" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>78</v>
+        <v>96</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>79</v>
+        <v>97</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>81</v>
+        <v>99</v>
+      </c>
+      <c r="H29" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="I29" s="0" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C32" s="0" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>82</v>
+        <v>101</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>83</v>
+        <v>102</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>84</v>
+        <v>103</v>
+      </c>
+      <c r="H32" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="I32" s="0" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C33" s="0" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>85</v>
+        <v>105</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>86</v>
+        <v>106</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>87</v>
+        <v>107</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>88</v>
+        <v>108</v>
+      </c>
+      <c r="H33" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="I33" s="0" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="0" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>89</v>
+        <v>110</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>90</v>
+        <v>111</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>91</v>
+        <v>112</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>92</v>
+        <v>113</v>
+      </c>
+      <c r="H34" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="I34" s="0" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C37" s="0" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>93</v>
+        <v>115</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>95</v>
+        <v>117</v>
+      </c>
+      <c r="H37" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="I37" s="0" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C38" s="0" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>96</v>
+        <v>119</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>97</v>
+        <v>120</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>98</v>
+        <v>121</v>
+      </c>
+      <c r="H38" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="I38" s="0" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C39" s="0" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>99</v>
+        <v>123</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>100</v>
+        <v>124</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>101</v>
+        <v>125</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>102</v>
+        <v>126</v>
+      </c>
+      <c r="H39" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="I39" s="0" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C41" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>103</v>
+        <v>128</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>104</v>
+        <v>129</v>
       </c>
       <c r="G41" s="0" t="s">
-        <v>105</v>
+        <v>130</v>
+      </c>
+      <c r="H41" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="I41" s="0" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -1679,8 +1903,8 @@
   </sheetPr>
   <dimension ref="A1:D58"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1694,688 +1918,688 @@
   <sheetData>
     <row r="1" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>106</v>
+        <v>132</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>107</v>
+        <v>133</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>108</v>
+        <v>134</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>109</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>110</v>
+        <v>136</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>111</v>
+        <v>137</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>112</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>113</v>
+        <v>139</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>114</v>
+        <v>140</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>114</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>115</v>
+        <v>141</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>116</v>
+        <v>142</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>117</v>
+        <v>143</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>118</v>
+        <v>144</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>119</v>
+        <v>145</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>120</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>121</v>
+        <v>147</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>122</v>
+        <v>148</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>123</v>
+        <v>149</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>124</v>
+        <v>150</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>125</v>
+        <v>151</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>126</v>
+        <v>152</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>127</v>
+        <v>153</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>128</v>
+        <v>154</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>129</v>
+        <v>155</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>130</v>
+        <v>156</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>131</v>
+        <v>157</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>132</v>
+        <v>158</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>133</v>
+        <v>159</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>134</v>
+        <v>160</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>135</v>
+        <v>161</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>136</v>
+        <v>162</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>137</v>
+        <v>163</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>138</v>
+        <v>164</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>139</v>
+        <v>165</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>140</v>
+        <v>166</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>141</v>
+        <v>167</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>142</v>
+        <v>168</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>143</v>
+        <v>169</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>144</v>
+        <v>170</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>145</v>
+        <v>171</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>146</v>
+        <v>172</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>147</v>
+        <v>173</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>148</v>
+        <v>174</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>149</v>
+        <v>175</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>150</v>
+        <v>176</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>151</v>
+        <v>177</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>152</v>
+        <v>178</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>153</v>
+        <v>179</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>154</v>
+        <v>180</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>155</v>
+        <v>181</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>156</v>
+        <v>182</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>157</v>
+        <v>183</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>158</v>
+        <v>184</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>159</v>
+        <v>185</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>160</v>
+        <v>186</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>161</v>
+        <v>187</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>162</v>
+        <v>188</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>163</v>
+        <v>189</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>164</v>
+        <v>190</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>165</v>
+        <v>191</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>166</v>
+        <v>192</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>167</v>
+        <v>193</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>168</v>
+        <v>194</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>169</v>
+        <v>195</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>171</v>
+        <v>197</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>172</v>
+        <v>198</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>173</v>
+        <v>199</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>174</v>
+        <v>200</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>175</v>
+        <v>201</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>176</v>
+        <v>202</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>177</v>
+        <v>203</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>178</v>
+        <v>204</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>179</v>
+        <v>205</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>180</v>
+        <v>206</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>181</v>
+        <v>207</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>182</v>
+        <v>208</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>183</v>
+        <v>209</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>185</v>
+        <v>211</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>186</v>
+        <v>212</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>187</v>
+        <v>213</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>188</v>
+        <v>214</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>174</v>
+        <v>200</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>175</v>
+        <v>201</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>189</v>
+        <v>215</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>190</v>
+        <v>216</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>191</v>
+        <v>217</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>192</v>
+        <v>218</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>193</v>
+        <v>219</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>194</v>
+        <v>220</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>194</v>
+        <v>220</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>195</v>
+        <v>221</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>196</v>
+        <v>222</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>197</v>
+        <v>223</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>198</v>
+        <v>224</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>199</v>
+        <v>225</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>200</v>
+        <v>226</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>201</v>
+        <v>227</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>202</v>
+        <v>228</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>203</v>
+        <v>229</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>78</v>
+        <v>96</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>204</v>
+        <v>230</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>205</v>
+        <v>231</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>205</v>
+        <v>231</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>78</v>
+        <v>96</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>206</v>
+        <v>232</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>207</v>
+        <v>233</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>208</v>
+        <v>234</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>78</v>
+        <v>96</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>209</v>
+        <v>235</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>210</v>
+        <v>236</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>211</v>
+        <v>237</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>85</v>
+        <v>105</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>212</v>
+        <v>238</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>213</v>
+        <v>239</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>214</v>
+        <v>240</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>85</v>
+        <v>105</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>215</v>
+        <v>241</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>216</v>
+        <v>242</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>217</v>
+        <v>243</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>85</v>
+        <v>105</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>171</v>
+        <v>197</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>218</v>
+        <v>244</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>214</v>
+        <v>240</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>89</v>
+        <v>110</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>219</v>
+        <v>245</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>220</v>
+        <v>246</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>221</v>
+        <v>247</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>89</v>
+        <v>110</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>222</v>
+        <v>248</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>223</v>
+        <v>249</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>224</v>
+        <v>250</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>89</v>
+        <v>110</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>171</v>
+        <v>197</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>225</v>
+        <v>251</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>226</v>
+        <v>252</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>89</v>
+        <v>110</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>174</v>
+        <v>200</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>175</v>
+        <v>201</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>176</v>
+        <v>202</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>99</v>
+        <v>123</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>227</v>
+        <v>253</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>228</v>
+        <v>254</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>229</v>
+        <v>255</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>99</v>
+        <v>123</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>230</v>
+        <v>256</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>231</v>
+        <v>257</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>232</v>
+        <v>258</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>99</v>
+        <v>123</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>171</v>
+        <v>197</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>233</v>
+        <v>259</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>234</v>
+        <v>260</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>99</v>
+        <v>123</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>174</v>
+        <v>200</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>175</v>
+        <v>201</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>189</v>
+        <v>215</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>99</v>
+        <v>123</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>198</v>
+        <v>224</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>199</v>
+        <v>225</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>200</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -2418,126 +2642,126 @@
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>235</v>
+        <v>261</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>236</v>
+        <v>262</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>237</v>
+        <v>263</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>238</v>
+        <v>264</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>239</v>
+        <v>265</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>240</v>
+        <v>266</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>241</v>
+        <v>267</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>242</v>
+        <v>268</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>243</v>
+        <v>269</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>244</v>
+        <v>270</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>245</v>
+        <v>271</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>246</v>
+        <v>272</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>247</v>
+        <v>273</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>248</v>
+        <v>274</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>248</v>
+        <v>274</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>249</v>
+        <v>275</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>250</v>
+        <v>276</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>251</v>
+        <v>277</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>252</v>
+        <v>278</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>252</v>
+        <v>278</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="45.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>253</v>
+        <v>279</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>254</v>
+        <v>280</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>255</v>
+        <v>281</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>252</v>
+        <v>278</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>252</v>
+        <v>278</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="64.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>253</v>
+        <v>279</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>254</v>
+        <v>280</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>256</v>
+        <v>282</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>252</v>
+        <v>278</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>252</v>
+        <v>278</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="62" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>253</v>
+        <v>279</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>257</v>
+        <v>283</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>258</v>
+        <v>284</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>252</v>
+        <v>278</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>252</v>
+        <v>278</v>
       </c>
     </row>
   </sheetData>
@@ -2558,8 +2782,8 @@
   </sheetPr>
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2572,54 +2796,54 @@
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>259</v>
+        <v>285</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>260</v>
+        <v>286</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>261</v>
+        <v>5</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>262</v>
+        <v>6</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>263</v>
+        <v>287</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>264</v>
+        <v>288</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>265</v>
+        <v>289</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>266</v>
+        <v>290</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>267</v>
+        <v>291</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>268</v>
+        <v>292</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>269</v>
+        <v>293</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>270</v>
+        <v>294</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>266</v>
+        <v>290</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>271</v>
+        <v>295</v>
       </c>
       <c r="B6" s="2" t="n">
         <f aca="false">TRUE()</f>
@@ -2628,40 +2852,40 @@
     </row>
     <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>272</v>
+        <v>296</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>273</v>
+        <v>297</v>
       </c>
       <c r="B8" s="7" t="n">
-        <v>20170715</v>
+        <v>20170717</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>274</v>
+        <v>298</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>275</v>
+        <v>299</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>276</v>
+        <v>300</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>277</v>
+        <v>301</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>278</v>
+        <v>302</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>279</v>
+        <v>303</v>
       </c>
     </row>
   </sheetData>
@@ -2693,138 +2917,138 @@
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>280</v>
+        <v>304</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>281</v>
+        <v>305</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>282</v>
+        <v>306</v>
       </c>
       <c r="D1" s="0" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>260</v>
+        <v>286</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>283</v>
+        <v>307</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>284</v>
+        <v>308</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>285</v>
+        <v>309</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>286</v>
+        <v>310</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>287</v>
+        <v>311</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>283</v>
+        <v>307</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>284</v>
+        <v>308</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>288</v>
+        <v>312</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>286</v>
+        <v>310</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>289</v>
+        <v>313</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>283</v>
+        <v>307</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>284</v>
+        <v>308</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>290</v>
+        <v>314</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>286</v>
+        <v>310</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>291</v>
+        <v>315</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>283</v>
+        <v>307</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>284</v>
+        <v>308</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>292</v>
+        <v>316</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>286</v>
+        <v>310</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>291</v>
+        <v>315</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>293</v>
+        <v>317</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>284</v>
+        <v>308</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>294</v>
+        <v>318</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>286</v>
+        <v>310</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>175</v>
+        <v>201</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>293</v>
+        <v>317</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>284</v>
+        <v>308</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>295</v>
+        <v>319</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>286</v>
+        <v>310</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>296</v>
+        <v>320</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>293</v>
+        <v>317</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>284</v>
+        <v>308</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>297</v>
+        <v>321</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>286</v>
+        <v>310</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>298</v>
+        <v>322</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change list view filename
</commit_message>
<xml_diff>
--- a/app/config/tables/health_facility/forms/health_facility/health_facility.xlsx
+++ b/app/config/tables/health_facility/forms/health_facility/health_facility.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="322">
   <si>
     <t xml:space="preserve">clause</t>
   </si>
@@ -969,6 +969,9 @@
   </si>
   <si>
     <t xml:space="preserve">mapListViewFileName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">config/assets/aa_health_facility_map.html</t>
   </si>
   <si>
     <t xml:space="preserve">TableMapFragment</t>
@@ -2776,7 +2779,7 @@
   </sheetPr>
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -2900,8 +2903,8 @@
   </sheetPr>
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2991,18 +2994,18 @@
         <v>308</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>306</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>308</v>
@@ -3013,36 +3016,36 @@
     </row>
     <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>306</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>308</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>306</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>308</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix translation in health facility form
</commit_message>
<xml_diff>
--- a/app/config/tables/health_facility/forms/health_facility/health_facility.xlsx
+++ b/app/config/tables/health_facility/forms/health_facility/health_facility.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="323">
   <si>
     <t xml:space="preserve">clause</t>
   </si>
@@ -749,10 +749,13 @@
     <t xml:space="preserve">Delivery</t>
   </si>
   <si>
+    <t xml:space="preserve">Envío</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Both Depot and Delivery</t>
+  </si>
+  <si>
     <t xml:space="preserve">Depósito y Envío</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Both Depot and Delivery</t>
   </si>
   <si>
     <t xml:space="preserve">static</t>
@@ -1900,8 +1903,8 @@
   </sheetPr>
   <dimension ref="A1:D58"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D47" activeCellId="0" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2470,7 +2473,7 @@
         <v>242</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2478,13 +2481,13 @@
         <v>110</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2492,13 +2495,13 @@
         <v>110</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2509,10 +2512,10 @@
         <v>195</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2534,13 +2537,13 @@
         <v>123</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2548,13 +2551,13 @@
         <v>123</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2565,10 +2568,10 @@
         <v>195</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2639,66 +2642,66 @@
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="26" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="45.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2706,19 +2709,19 @@
         <v>27</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>278</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="J3" s="0" t="s">
         <v>277</v>
       </c>
-      <c r="H3" s="0" t="s">
-        <v>278</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="J3" s="0" t="s">
-        <v>276</v>
-      </c>
       <c r="K3" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="64.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2726,19 +2729,19 @@
         <v>32</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>278</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="J4" s="0" t="s">
         <v>277</v>
       </c>
-      <c r="H4" s="0" t="s">
-        <v>278</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="J4" s="0" t="s">
-        <v>276</v>
-      </c>
       <c r="K4" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="62" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2746,19 +2749,19 @@
         <v>38</v>
       </c>
       <c r="B5" s="0" t="s">
+        <v>278</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>282</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="J5" s="0" t="s">
         <v>277</v>
       </c>
-      <c r="H5" s="0" t="s">
-        <v>281</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="J5" s="0" t="s">
-        <v>276</v>
-      </c>
       <c r="K5" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
   </sheetData>
@@ -2793,10 +2796,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>5</v>
@@ -2805,42 +2808,42 @@
         <v>6</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B6" s="2" t="n">
         <f aca="false">TRUE()</f>
@@ -2849,7 +2852,7 @@
     </row>
     <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>13</v>
@@ -2857,7 +2860,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B8" s="7" t="n">
         <v>20170718</v>
@@ -2865,24 +2868,24 @@
     </row>
     <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
   </sheetData>
@@ -2903,7 +2906,7 @@
   </sheetPr>
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -2914,101 +2917,101 @@
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="D1" s="0" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="E6" s="0" t="s">
         <v>199</v>
@@ -3016,36 +3019,36 @@
     </row>
     <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix health facility list view and add temp hack for list view logic and count
</commit_message>
<xml_diff>
--- a/app/config/tables/health_facility/forms/health_facility/health_facility.xlsx
+++ b/app/config/tables/health_facility/forms/health_facility/health_facility.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33920" windowHeight="20000" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="8440" yWindow="2360" windowWidth="31600" windowHeight="16100" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="324">
   <si>
     <t>clause</t>
   </si>
@@ -996,6 +996,9 @@
   </si>
   <si>
     <t>config/tables/health_facility/html/health_facility_list.html</t>
+  </si>
+  <si>
+    <t>config/tables/health_facility/html/hFacility_list.html</t>
   </si>
 </sst>
 </file>
@@ -3116,7 +3119,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3208,7 +3211,7 @@
         <v>296</v>
       </c>
       <c r="E5" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="6" spans="1:5">

</xml_diff>

<commit_message>
Modify health_facility as necessary
</commit_message>
<xml_diff>
--- a/app/config/tables/health_facility/forms/health_facility/health_facility.xlsx
+++ b/app/config/tables/health_facility/forms/health_facility/health_facility.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clarice\cold-chain\cold-chain-app-designer\app\config\tables\health_facility\forms\health_facility\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2500" yWindow="0" windowWidth="33300" windowHeight="18360" tabRatio="500"/>
+    <workbookView xWindow="2500" yWindow="0" windowWidth="9000" windowHeight="0" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -14,7 +19,7 @@
     <sheet name="properties" sheetId="5" r:id="rId5"/>
     <sheet name="model" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="162913" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="344">
   <si>
     <t>clause</t>
   </si>
@@ -161,33 +166,9 @@
     <t>integer</t>
   </si>
   <si>
-    <t>facility_population</t>
-  </si>
-  <si>
-    <t>Facility Population</t>
-  </si>
-  <si>
-    <t>Población de facilidad</t>
-  </si>
-  <si>
-    <t>Enter the facility population</t>
-  </si>
-  <si>
     <t>decimal</t>
   </si>
   <si>
-    <t>facility_coverage</t>
-  </si>
-  <si>
-    <t>Facility Coverage</t>
-  </si>
-  <si>
-    <t>Cobertura (porcentaje)</t>
-  </si>
-  <si>
-    <t>Percent coverage?</t>
-  </si>
-  <si>
     <t>elec_sources</t>
   </si>
   <si>
@@ -227,78 +208,15 @@
     <t>fuel_availability</t>
   </si>
   <si>
-    <t>gas_availability</t>
-  </si>
-  <si>
-    <t>Gas Availability</t>
-  </si>
-  <si>
     <t>Disponibilidad de combustible</t>
   </si>
   <si>
-    <t>Choose the gas availability</t>
-  </si>
-  <si>
-    <t>kerosene_availability</t>
-  </si>
-  <si>
-    <t>Kerosene Availability</t>
-  </si>
-  <si>
-    <t>Disponibilidad de queroseno</t>
-  </si>
-  <si>
-    <t>Choose the kerosene availability</t>
-  </si>
-  <si>
     <t>yes_no</t>
   </si>
   <si>
-    <t>solar_suitable_climate</t>
-  </si>
-  <si>
-    <t>Solar Suitable Climate</t>
-  </si>
-  <si>
-    <t>Clima adecuedo por energía solár</t>
-  </si>
-  <si>
-    <t>Is this a solar suitable climate?</t>
-  </si>
-  <si>
-    <t>¿Es la clima adecuedo por energía solár?</t>
-  </si>
-  <si>
-    <t>solar_suitable_site</t>
-  </si>
-  <si>
-    <t>Solar Suitable Site</t>
-  </si>
-  <si>
-    <t>Facilidad adecuedo por energía solar</t>
-  </si>
-  <si>
-    <t>Is this a solar suitable site?</t>
-  </si>
-  <si>
-    <t>¿Es la facilidad adecuedo por energía solár?</t>
-  </si>
-  <si>
     <t>climate_types</t>
   </si>
   <si>
-    <t>climate_zone</t>
-  </si>
-  <si>
-    <t>Climate Zone</t>
-  </si>
-  <si>
-    <t>Clima de ubicación</t>
-  </si>
-  <si>
-    <t>What is the climate of this location?</t>
-  </si>
-  <si>
     <t>distance_to_supply</t>
   </si>
   <si>
@@ -314,27 +232,6 @@
     <t>storage_types</t>
   </si>
   <si>
-    <t>storage_type</t>
-  </si>
-  <si>
-    <t>Storage Type</t>
-  </si>
-  <si>
-    <t>Tipo de almacenamiento</t>
-  </si>
-  <si>
-    <t>Storage type?</t>
-  </si>
-  <si>
-    <t>delivery_types</t>
-  </si>
-  <si>
-    <t>delivery_type</t>
-  </si>
-  <si>
-    <t>Delivery Type</t>
-  </si>
-  <si>
     <t>Tipo de envío</t>
   </si>
   <si>
@@ -350,21 +247,6 @@
     <t>Intervalo de reabastecimiento</t>
   </si>
   <si>
-    <t>Vaccine Supply Interval?</t>
-  </si>
-  <si>
-    <t>vaccine_reserve_stock_requirement</t>
-  </si>
-  <si>
-    <t>Minimum Reserve Requirement</t>
-  </si>
-  <si>
-    <t>Tamaño Minimo de Reserva</t>
-  </si>
-  <si>
-    <t>Vaccine Reserve Stock Requirement?</t>
-  </si>
-  <si>
     <t>vaccine_modes</t>
   </si>
   <si>
@@ -731,12 +613,6 @@
     <t>static</t>
   </si>
   <si>
-    <t>Static</t>
-  </si>
-  <si>
-    <t>Estático</t>
-  </si>
-  <si>
     <t>outreach</t>
   </si>
   <si>
@@ -999,13 +875,202 @@
   </si>
   <si>
     <t>(selected(data('electricity_source'), 'grid') || selected(data('electricity_source'), 'both'))</t>
+  </si>
+  <si>
+    <t>contact_title</t>
+  </si>
+  <si>
+    <t>Contact Title</t>
+  </si>
+  <si>
+    <t>contact_phone_number</t>
+  </si>
+  <si>
+    <t>Contact Phone Number</t>
+  </si>
+  <si>
+    <t>Number of cold boxes at facility</t>
+  </si>
+  <si>
+    <t>Number of vaccine carriers at facility</t>
+  </si>
+  <si>
+    <t>Number of freeze safe cold boxes at facility</t>
+  </si>
+  <si>
+    <t>Number of freeze safe vaccine carriers at facility</t>
+  </si>
+  <si>
+    <t>number_of_cold_boxes</t>
+  </si>
+  <si>
+    <t>number_of_vaccine_carriers</t>
+  </si>
+  <si>
+    <t>number_of_fs_cold_boxes</t>
+  </si>
+  <si>
+    <t>number_of_fs_vaccine_carriers</t>
+  </si>
+  <si>
+    <t>Título del contacto</t>
+  </si>
+  <si>
+    <t>Contact Title?</t>
+  </si>
+  <si>
+    <t>Título del contacto?</t>
+  </si>
+  <si>
+    <t>Teléfono de contacto</t>
+  </si>
+  <si>
+    <t>Teléfono de contacto?</t>
+  </si>
+  <si>
+    <t>Number of cold boxes at facility?</t>
+  </si>
+  <si>
+    <t>Number of vaccine carriers at facility?</t>
+  </si>
+  <si>
+    <t>Number of freeze safe cold boxes at facility?</t>
+  </si>
+  <si>
+    <t>Number of freeze safe vaccine carriers at facility?</t>
+  </si>
+  <si>
+    <t>Número de cajas frías en la facilidad</t>
+  </si>
+  <si>
+    <t>Número de portadores de vacunas en la facilidad</t>
+  </si>
+  <si>
+    <t>Número de cajas frías en la facilidad?</t>
+  </si>
+  <si>
+    <t>Número de portadores de vacunas en la facilidad?</t>
+  </si>
+  <si>
+    <t>Número de cajas frías a congelación segura en la facilidad</t>
+  </si>
+  <si>
+    <t>Número de cajas frías a congelación segura en la facilidad?</t>
+  </si>
+  <si>
+    <t>Número de portadores de vacunas a congelación segura en la facilidad</t>
+  </si>
+  <si>
+    <t>Número de portadores de vacunas a congelación segura en la facilidad?</t>
+  </si>
+  <si>
+    <t>catchment_population</t>
+  </si>
+  <si>
+    <t>Catchment Population</t>
+  </si>
+  <si>
+    <t>Captación de facilidad</t>
+  </si>
+  <si>
+    <t>Enter the catchment population</t>
+  </si>
+  <si>
+    <t>Immunization_services_offered</t>
+  </si>
+  <si>
+    <t>Immunization Services Offered</t>
+  </si>
+  <si>
+    <t>immunization_services</t>
+  </si>
+  <si>
+    <t>fuel_availability_types</t>
+  </si>
+  <si>
+    <t>Fuel Availability</t>
+  </si>
+  <si>
+    <t>Choose the fuel availability</t>
+  </si>
+  <si>
+    <t>Vaccine Supply Interval (# of weeks between supply)?</t>
+  </si>
+  <si>
+    <t>Tipo de envío?</t>
+  </si>
+  <si>
+    <t>Intervalo de reabastecimiento (# de semanas entre el suministro)?</t>
+  </si>
+  <si>
+    <t>Modo de recibir vacunas?</t>
+  </si>
+  <si>
+    <t>Nombre del contacto?</t>
+  </si>
+  <si>
+    <t>Distancia al más proximo punto de reabastecimiento?</t>
+  </si>
+  <si>
+    <t>health_station</t>
+  </si>
+  <si>
+    <t>Health Station</t>
+  </si>
+  <si>
+    <t>Estación de salud</t>
+  </si>
+  <si>
+    <t>solar</t>
+  </si>
+  <si>
+    <t>Solar</t>
+  </si>
+  <si>
+    <t>both_grid_and_generator</t>
+  </si>
+  <si>
+    <t>both_grid_and_solar</t>
+  </si>
+  <si>
+    <t>Both Grid and Solar</t>
+  </si>
+  <si>
+    <t>both_solar_and_generator</t>
+  </si>
+  <si>
+    <t>Red y solar</t>
+  </si>
+  <si>
+    <t>both_static_and_outreach</t>
+  </si>
+  <si>
+    <t>Static/Fixed Post</t>
+  </si>
+  <si>
+    <t>storage_only</t>
+  </si>
+  <si>
+    <t>Storage Only</t>
+  </si>
+  <si>
+    <t>Solo almacenamiento</t>
+  </si>
+  <si>
+    <t>Estático/Puesto Fijo</t>
+  </si>
+  <si>
+    <t>Both Generator and Solar</t>
+  </si>
+  <si>
+    <t>Generador y solar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -1043,6 +1108,19 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF222222"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1058,12 +1136,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -1076,7 +1169,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1097,6 +1190,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -1178,6 +1279,14 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1503,25 +1612,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K39"/>
+  <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="C22" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="25.6640625" customWidth="1"/>
     <col min="2" max="2" width="49" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="18.33203125" customWidth="1"/>
     <col min="5" max="5" width="20.6640625" customWidth="1"/>
-    <col min="6" max="8" width="26.83203125" customWidth="1"/>
+    <col min="6" max="6" width="43.25" customWidth="1"/>
+    <col min="7" max="8" width="26.83203125" customWidth="1"/>
     <col min="9" max="10" width="47.6640625" customWidth="1"/>
     <col min="11" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1556,7 +1666,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1570,7 +1680,7 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:11" ht="25" customHeight="1">
+    <row r="3" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
@@ -1596,7 +1706,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C4" t="s">
         <v>12</v>
       </c>
@@ -1620,17 +1730,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C7" t="s">
         <v>22</v>
       </c>
@@ -1650,7 +1760,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C8" t="s">
         <v>26</v>
       </c>
@@ -1679,17 +1789,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C11" t="s">
         <v>32</v>
       </c>
@@ -1712,7 +1822,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C12" t="s">
         <v>32</v>
       </c>
@@ -1735,417 +1845,414 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C13" t="s">
         <v>43</v>
       </c>
       <c r="E13" t="s">
-        <v>44</v>
+        <v>310</v>
       </c>
       <c r="F13" t="s">
+        <v>311</v>
+      </c>
+      <c r="G13" t="s">
+        <v>312</v>
+      </c>
+      <c r="H13" t="s">
+        <v>313</v>
+      </c>
+      <c r="I13" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" t="s">
         <v>45</v>
       </c>
-      <c r="G13" t="s">
+      <c r="E16" t="s">
         <v>46</v>
       </c>
-      <c r="H13" t="s">
+      <c r="F16" t="s">
         <v>47</v>
       </c>
-      <c r="I13" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
-      <c r="C14" t="s">
+      <c r="G16" t="s">
         <v>48</v>
       </c>
-      <c r="E14" t="s">
+      <c r="H16" t="s">
         <v>49</v>
       </c>
-      <c r="F14" t="s">
+      <c r="I16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>50</v>
       </c>
-      <c r="G14" t="s">
+      <c r="B17" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" t="s">
         <v>51</v>
       </c>
-      <c r="H14" t="s">
+      <c r="E18" t="s">
         <v>52</v>
       </c>
-      <c r="I14" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11">
-      <c r="A15" t="s">
+      <c r="F18" t="s">
+        <v>53</v>
+      </c>
+      <c r="G18" t="s">
+        <v>54</v>
+      </c>
+      <c r="H18" t="s">
+        <v>55</v>
+      </c>
+      <c r="I18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C20" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" t="s">
+        <v>317</v>
+      </c>
+      <c r="E20" t="s">
+        <v>57</v>
+      </c>
+      <c r="F20" t="s">
+        <v>318</v>
+      </c>
+      <c r="G20" t="s">
+        <v>58</v>
+      </c>
+      <c r="H20" t="s">
+        <v>319</v>
+      </c>
+      <c r="I20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
-      <c r="A16" t="s">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
-      <c r="C17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D17" t="s">
-        <v>53</v>
-      </c>
-      <c r="E17" t="s">
-        <v>54</v>
-      </c>
-      <c r="F17" t="s">
-        <v>55</v>
-      </c>
-      <c r="G17" t="s">
-        <v>56</v>
-      </c>
-      <c r="H17" t="s">
-        <v>57</v>
-      </c>
-      <c r="I17" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
-      <c r="A18" t="s">
-        <v>58</v>
-      </c>
-      <c r="B18" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="C19" t="s">
-        <v>32</v>
-      </c>
-      <c r="D19" t="s">
-        <v>59</v>
-      </c>
-      <c r="E19" t="s">
-        <v>60</v>
-      </c>
-      <c r="F19" t="s">
-        <v>61</v>
-      </c>
-      <c r="G19" t="s">
-        <v>62</v>
-      </c>
-      <c r="H19" t="s">
-        <v>63</v>
-      </c>
-      <c r="I19" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
-      <c r="A20" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="C21" t="s">
-        <v>32</v>
-      </c>
-      <c r="D21" t="s">
-        <v>65</v>
-      </c>
-      <c r="E21" t="s">
-        <v>66</v>
-      </c>
-      <c r="F21" t="s">
-        <v>67</v>
-      </c>
-      <c r="G21" t="s">
-        <v>68</v>
-      </c>
-      <c r="H21" t="s">
-        <v>69</v>
-      </c>
-      <c r="I21" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
-      <c r="C22" t="s">
-        <v>32</v>
-      </c>
-      <c r="D22" t="s">
-        <v>65</v>
-      </c>
-      <c r="E22" t="s">
-        <v>70</v>
-      </c>
-      <c r="F22" t="s">
-        <v>71</v>
-      </c>
-      <c r="G22" t="s">
-        <v>72</v>
-      </c>
-      <c r="H22" t="s">
-        <v>73</v>
-      </c>
-      <c r="I22" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C25" t="s">
-        <v>32</v>
-      </c>
-      <c r="D25" t="s">
-        <v>74</v>
+        <v>44</v>
       </c>
       <c r="E25" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="F25" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="G25" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="H25" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="I25" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C26" t="s">
         <v>32</v>
       </c>
       <c r="D26" t="s">
+        <v>316</v>
+      </c>
+      <c r="E26" t="s">
+        <v>314</v>
+      </c>
+      <c r="F26" t="s">
+        <v>315</v>
+      </c>
+      <c r="G26" t="s">
+        <v>66</v>
+      </c>
+      <c r="H26" t="s">
+        <v>67</v>
+      </c>
+      <c r="I26" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C29" t="s">
+        <v>43</v>
+      </c>
+      <c r="E29" t="s">
+        <v>68</v>
+      </c>
+      <c r="F29" t="s">
+        <v>69</v>
+      </c>
+      <c r="G29" t="s">
+        <v>70</v>
+      </c>
+      <c r="H29" t="s">
+        <v>320</v>
+      </c>
+      <c r="I29" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C30" t="s">
+        <v>32</v>
+      </c>
+      <c r="D30" t="s">
+        <v>71</v>
+      </c>
+      <c r="E30" t="s">
+        <v>72</v>
+      </c>
+      <c r="F30" t="s">
+        <v>73</v>
+      </c>
+      <c r="G30" t="s">
         <v>74</v>
       </c>
-      <c r="E26" t="s">
-        <v>80</v>
-      </c>
-      <c r="F26" t="s">
-        <v>81</v>
-      </c>
-      <c r="G26" t="s">
-        <v>82</v>
-      </c>
-      <c r="H26" t="s">
-        <v>83</v>
-      </c>
-      <c r="I26" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
-      <c r="C27" t="s">
-        <v>32</v>
-      </c>
-      <c r="D27" t="s">
-        <v>85</v>
-      </c>
-      <c r="E27" t="s">
-        <v>86</v>
-      </c>
-      <c r="F27" t="s">
-        <v>87</v>
-      </c>
-      <c r="G27" t="s">
-        <v>88</v>
-      </c>
-      <c r="H27" t="s">
-        <v>89</v>
-      </c>
-      <c r="I27" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9">
-      <c r="A28" t="s">
+      <c r="H30" t="s">
+        <v>75</v>
+      </c>
+      <c r="I30" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
-      <c r="A29" t="s">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
-      <c r="C30" t="s">
-        <v>48</v>
-      </c>
-      <c r="E30" t="s">
-        <v>90</v>
-      </c>
-      <c r="F30" t="s">
-        <v>91</v>
-      </c>
-      <c r="G30" t="s">
-        <v>92</v>
-      </c>
-      <c r="H30" t="s">
-        <v>93</v>
-      </c>
-      <c r="I30" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9">
-      <c r="C31" t="s">
-        <v>32</v>
-      </c>
-      <c r="D31" t="s">
-        <v>94</v>
-      </c>
-      <c r="E31" t="s">
-        <v>95</v>
-      </c>
-      <c r="F31" t="s">
-        <v>96</v>
-      </c>
-      <c r="G31" t="s">
-        <v>97</v>
-      </c>
-      <c r="H31" t="s">
-        <v>98</v>
-      </c>
-      <c r="I31" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9">
-      <c r="C32" t="s">
-        <v>32</v>
-      </c>
-      <c r="D32" t="s">
-        <v>99</v>
-      </c>
-      <c r="E32" t="s">
-        <v>100</v>
-      </c>
-      <c r="F32" t="s">
-        <v>101</v>
-      </c>
-      <c r="G32" t="s">
-        <v>102</v>
-      </c>
-      <c r="H32" t="s">
-        <v>103</v>
-      </c>
-      <c r="I32" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9">
-      <c r="A33" t="s">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C33" t="s">
+        <v>12</v>
+      </c>
+      <c r="E33" t="s">
+        <v>76</v>
+      </c>
+      <c r="F33" t="s">
+        <v>77</v>
+      </c>
+      <c r="G33" t="s">
+        <v>78</v>
+      </c>
+      <c r="H33" t="s">
+        <v>79</v>
+      </c>
+      <c r="I33" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C34" t="s">
+        <v>12</v>
+      </c>
+      <c r="E34" t="s">
+        <v>281</v>
+      </c>
+      <c r="F34" t="s">
+        <v>282</v>
+      </c>
+      <c r="G34" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="H34" t="s">
+        <v>294</v>
+      </c>
+      <c r="I34" s="10" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C35" t="s">
+        <v>12</v>
+      </c>
+      <c r="E35" t="s">
+        <v>283</v>
+      </c>
+      <c r="F35" t="s">
+        <v>284</v>
+      </c>
+      <c r="G35" s="11" t="s">
+        <v>296</v>
+      </c>
+      <c r="H35" t="s">
+        <v>284</v>
+      </c>
+      <c r="I35" s="11" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
-      <c r="A34" t="s">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
-      <c r="C35" t="s">
+    <row r="38" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C38" t="s">
         <v>43</v>
       </c>
-      <c r="E35" t="s">
-        <v>104</v>
-      </c>
-      <c r="F35" t="s">
-        <v>105</v>
-      </c>
-      <c r="G35" t="s">
-        <v>106</v>
-      </c>
-      <c r="H35" t="s">
-        <v>107</v>
-      </c>
-      <c r="I35" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9">
-      <c r="C36" t="s">
+      <c r="E38" t="s">
+        <v>289</v>
+      </c>
+      <c r="F38" t="s">
+        <v>285</v>
+      </c>
+      <c r="G38" s="11" t="s">
+        <v>302</v>
+      </c>
+      <c r="H38" t="s">
+        <v>298</v>
+      </c>
+      <c r="I38" s="11" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C39" t="s">
         <v>43</v>
       </c>
-      <c r="E36" t="s">
-        <v>108</v>
-      </c>
-      <c r="F36" t="s">
-        <v>109</v>
-      </c>
-      <c r="G36" t="s">
-        <v>110</v>
-      </c>
-      <c r="H36" t="s">
-        <v>111</v>
-      </c>
-      <c r="I36" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9">
-      <c r="C37" t="s">
-        <v>32</v>
-      </c>
-      <c r="D37" t="s">
-        <v>112</v>
-      </c>
-      <c r="E37" t="s">
-        <v>113</v>
-      </c>
-      <c r="F37" t="s">
-        <v>114</v>
-      </c>
-      <c r="G37" t="s">
-        <v>115</v>
-      </c>
-      <c r="H37" t="s">
-        <v>116</v>
-      </c>
-      <c r="I37" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9">
-      <c r="A38" t="s">
+      <c r="E39" t="s">
+        <v>290</v>
+      </c>
+      <c r="F39" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="G39" s="12" t="s">
+        <v>303</v>
+      </c>
+      <c r="H39" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="I39" s="12" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A40" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="39" spans="1:9">
-      <c r="C39" t="s">
-        <v>12</v>
-      </c>
-      <c r="E39" t="s">
-        <v>117</v>
-      </c>
-      <c r="F39" t="s">
-        <v>118</v>
-      </c>
-      <c r="G39" t="s">
-        <v>119</v>
-      </c>
-      <c r="H39" t="s">
-        <v>120</v>
-      </c>
-      <c r="I39" t="s">
-        <v>119</v>
+      <c r="F40" s="9"/>
+    </row>
+    <row r="41" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A41" t="s">
+        <v>11</v>
+      </c>
+      <c r="F41" s="9"/>
+    </row>
+    <row r="42" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C42" t="s">
+        <v>43</v>
+      </c>
+      <c r="E42" t="s">
+        <v>291</v>
+      </c>
+      <c r="F42" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="G42" s="12" t="s">
+        <v>306</v>
+      </c>
+      <c r="H42" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="I42" s="12" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C43" t="s">
+        <v>43</v>
+      </c>
+      <c r="E43" t="s">
+        <v>292</v>
+      </c>
+      <c r="F43" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="G43" s="12" t="s">
+        <v>308</v>
+      </c>
+      <c r="H43" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="I43" s="12" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2156,13 +2263,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D58"/>
+  <dimension ref="A1:D63"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView topLeftCell="A8" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="23.1640625" customWidth="1"/>
     <col min="2" max="2" width="24.5" customWidth="1"/>
@@ -2171,12 +2278,12 @@
     <col min="5" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="20" customHeight="1">
+    <row r="1" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>121</v>
+        <v>80</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>122</v>
+        <v>81</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>5</v>
@@ -2185,681 +2292,751 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="B2" t="s">
-        <v>123</v>
+        <v>82</v>
       </c>
       <c r="C2" t="s">
-        <v>124</v>
+        <v>83</v>
       </c>
       <c r="D2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="B3" t="s">
-        <v>126</v>
+        <v>85</v>
       </c>
       <c r="C3" t="s">
-        <v>127</v>
+        <v>86</v>
       </c>
       <c r="D3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>128</v>
+        <v>87</v>
       </c>
       <c r="C5" t="s">
-        <v>129</v>
+        <v>88</v>
       </c>
       <c r="D5" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>131</v>
+        <v>90</v>
       </c>
       <c r="C6" t="s">
-        <v>132</v>
+        <v>91</v>
       </c>
       <c r="D6" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>134</v>
+        <v>93</v>
       </c>
       <c r="C7" t="s">
-        <v>135</v>
+        <v>94</v>
       </c>
       <c r="D7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>33</v>
       </c>
       <c r="B8" t="s">
-        <v>137</v>
+        <v>96</v>
       </c>
       <c r="C8" t="s">
-        <v>138</v>
+        <v>97</v>
       </c>
       <c r="D8" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>33</v>
       </c>
       <c r="B9" t="s">
-        <v>140</v>
+        <v>99</v>
       </c>
       <c r="C9" t="s">
-        <v>141</v>
+        <v>100</v>
       </c>
       <c r="D9" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>33</v>
       </c>
       <c r="B10" t="s">
-        <v>143</v>
+        <v>102</v>
       </c>
       <c r="C10" t="s">
-        <v>144</v>
+        <v>103</v>
       </c>
       <c r="D10" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>33</v>
       </c>
       <c r="B11" t="s">
-        <v>146</v>
+        <v>105</v>
       </c>
       <c r="C11" t="s">
-        <v>147</v>
+        <v>106</v>
       </c>
       <c r="D11" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>149</v>
+        <v>108</v>
       </c>
       <c r="C12" t="s">
-        <v>150</v>
+        <v>109</v>
       </c>
       <c r="D12" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>33</v>
       </c>
       <c r="B13" t="s">
-        <v>152</v>
+        <v>111</v>
       </c>
       <c r="C13" t="s">
-        <v>153</v>
+        <v>112</v>
       </c>
       <c r="D13" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="17" customHeight="1">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>33</v>
       </c>
       <c r="B14" t="s">
-        <v>155</v>
+        <v>114</v>
       </c>
       <c r="C14" t="s">
-        <v>156</v>
+        <v>115</v>
       </c>
       <c r="D14" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="17" customHeight="1">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>33</v>
       </c>
       <c r="B15" t="s">
-        <v>158</v>
+        <v>326</v>
       </c>
       <c r="C15" t="s">
-        <v>159</v>
-      </c>
-      <c r="D15" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
+        <v>327</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>33</v>
       </c>
       <c r="B16" t="s">
-        <v>161</v>
+        <v>117</v>
       </c>
       <c r="C16" t="s">
-        <v>162</v>
+        <v>118</v>
       </c>
       <c r="D16" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" t="s">
-        <v>164</v>
-      </c>
-      <c r="C18" t="s">
-        <v>165</v>
-      </c>
-      <c r="D18" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" t="s">
+        <v>120</v>
+      </c>
+      <c r="C17" t="s">
+        <v>121</v>
+      </c>
+      <c r="D17" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>38</v>
       </c>
       <c r="B19" t="s">
-        <v>167</v>
+        <v>123</v>
       </c>
       <c r="C19" t="s">
-        <v>168</v>
+        <v>124</v>
       </c>
       <c r="D19" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>38</v>
       </c>
       <c r="B20" t="s">
-        <v>170</v>
+        <v>126</v>
       </c>
       <c r="C20" t="s">
-        <v>171</v>
+        <v>127</v>
       </c>
       <c r="D20" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>38</v>
       </c>
       <c r="B21" t="s">
-        <v>173</v>
+        <v>129</v>
       </c>
       <c r="C21" t="s">
-        <v>174</v>
+        <v>130</v>
       </c>
       <c r="D21" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>38</v>
       </c>
       <c r="B22" t="s">
+        <v>132</v>
+      </c>
+      <c r="C22" t="s">
+        <v>133</v>
+      </c>
+      <c r="D22" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" t="s">
+        <v>135</v>
+      </c>
+      <c r="C23" t="s">
+        <v>136</v>
+      </c>
+      <c r="D23" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" t="s">
+        <v>138</v>
+      </c>
+      <c r="D25" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>45</v>
+      </c>
+      <c r="B26" t="s">
+        <v>329</v>
+      </c>
+      <c r="C26" t="s">
+        <v>330</v>
+      </c>
+      <c r="D26" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>45</v>
+      </c>
+      <c r="B27" t="s">
+        <v>140</v>
+      </c>
+      <c r="C27" t="s">
+        <v>141</v>
+      </c>
+      <c r="D27" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" t="s">
+        <v>331</v>
+      </c>
+      <c r="C28" t="s">
+        <v>144</v>
+      </c>
+      <c r="D28" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29" t="s">
+        <v>332</v>
+      </c>
+      <c r="C29" t="s">
+        <v>333</v>
+      </c>
+      <c r="D29" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>45</v>
+      </c>
+      <c r="B30" t="s">
+        <v>334</v>
+      </c>
+      <c r="C30" t="s">
+        <v>342</v>
+      </c>
+      <c r="D30" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>45</v>
+      </c>
+      <c r="B31" t="s">
+        <v>146</v>
+      </c>
+      <c r="C31" t="s">
+        <v>147</v>
+      </c>
+      <c r="D31" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>51</v>
+      </c>
+      <c r="B33" t="s">
+        <v>149</v>
+      </c>
+      <c r="C33" t="s">
+        <v>150</v>
+      </c>
+      <c r="D33" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>51</v>
+      </c>
+      <c r="B34" t="s">
+        <v>152</v>
+      </c>
+      <c r="C34" t="s">
+        <v>153</v>
+      </c>
+      <c r="D34" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>51</v>
+      </c>
+      <c r="B35" t="s">
+        <v>155</v>
+      </c>
+      <c r="C35" t="s">
+        <v>156</v>
+      </c>
+      <c r="D35" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>51</v>
+      </c>
+      <c r="B36" t="s">
+        <v>158</v>
+      </c>
+      <c r="C36" t="s">
+        <v>159</v>
+      </c>
+      <c r="D36" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>51</v>
+      </c>
+      <c r="B37" t="s">
+        <v>146</v>
+      </c>
+      <c r="C37" t="s">
+        <v>147</v>
+      </c>
+      <c r="D37" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>317</v>
+      </c>
+      <c r="B39" t="s">
+        <v>162</v>
+      </c>
+      <c r="C39" t="s">
+        <v>163</v>
+      </c>
+      <c r="D39" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>317</v>
+      </c>
+      <c r="B40" t="s">
+        <v>165</v>
+      </c>
+      <c r="C40" t="s">
+        <v>166</v>
+      </c>
+      <c r="D40" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>317</v>
+      </c>
+      <c r="B41" t="s">
+        <v>167</v>
+      </c>
+      <c r="C41" t="s">
+        <v>168</v>
+      </c>
+      <c r="D41" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>317</v>
+      </c>
+      <c r="B42" t="s">
+        <v>170</v>
+      </c>
+      <c r="C42" t="s">
+        <v>171</v>
+      </c>
+      <c r="D42" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>317</v>
+      </c>
+      <c r="B43" t="s">
+        <v>173</v>
+      </c>
+      <c r="C43" t="s">
+        <v>174</v>
+      </c>
+      <c r="D43" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>60</v>
+      </c>
+      <c r="B45" t="s">
         <v>176</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C45" t="s">
         <v>177</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D45" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>60</v>
+      </c>
+      <c r="B46" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" t="s">
-        <v>53</v>
-      </c>
-      <c r="B24" t="s">
-        <v>59</v>
-      </c>
-      <c r="C24" t="s">
+      <c r="C46" t="s">
         <v>179</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D46" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
-      <c r="A25" t="s">
-        <v>53</v>
-      </c>
-      <c r="B25" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>60</v>
+      </c>
+      <c r="B47" t="s">
         <v>181</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C47" t="s">
         <v>182</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D47" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
-      <c r="A26" t="s">
-        <v>53</v>
-      </c>
-      <c r="B26" t="s">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>65</v>
+      </c>
+      <c r="B49" t="s">
         <v>184</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C49" t="s">
         <v>185</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D49" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
-      <c r="A27" t="s">
-        <v>53</v>
-      </c>
-      <c r="B27" t="s">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>65</v>
+      </c>
+      <c r="B50" t="s">
         <v>187</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C50" t="s">
         <v>188</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D50" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
-      <c r="A29" t="s">
-        <v>59</v>
-      </c>
-      <c r="B29" t="s">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>65</v>
+      </c>
+      <c r="B51" t="s">
+        <v>143</v>
+      </c>
+      <c r="C51" t="s">
         <v>190</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D51" t="s">
         <v>191</v>
       </c>
-      <c r="D29" t="s">
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>316</v>
+      </c>
+      <c r="B53" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" t="s">
-        <v>59</v>
-      </c>
-      <c r="B30" t="s">
+      <c r="C53" t="s">
+        <v>337</v>
+      </c>
+      <c r="D53" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>316</v>
+      </c>
+      <c r="B54" t="s">
         <v>193</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C54" t="s">
         <v>194</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D54" s="1" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
-      <c r="A31" t="s">
-        <v>59</v>
-      </c>
-      <c r="B31" t="s">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>316</v>
+      </c>
+      <c r="B55" t="s">
+        <v>336</v>
+      </c>
+      <c r="C55" t="s">
         <v>196</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D55" t="s">
         <v>197</v>
       </c>
-      <c r="D31" t="s">
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>316</v>
+      </c>
+      <c r="B56" t="s">
+        <v>338</v>
+      </c>
+      <c r="C56" t="s">
+        <v>339</v>
+      </c>
+      <c r="D56" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>316</v>
+      </c>
+      <c r="B57" t="s">
+        <v>146</v>
+      </c>
+      <c r="C57" t="s">
+        <v>147</v>
+      </c>
+      <c r="D57" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>71</v>
+      </c>
+      <c r="B59" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" t="s">
-        <v>59</v>
-      </c>
-      <c r="B32" t="s">
+      <c r="C59" t="s">
         <v>199</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D59" t="s">
         <v>200</v>
       </c>
-      <c r="D32" t="s">
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>71</v>
+      </c>
+      <c r="B60" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" t="s">
-        <v>59</v>
-      </c>
-      <c r="B33" t="s">
-        <v>187</v>
-      </c>
-      <c r="C33" t="s">
-        <v>188</v>
-      </c>
-      <c r="D33" t="s">
+      <c r="C60" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" t="s">
-        <v>65</v>
-      </c>
-      <c r="B35" t="s">
+      <c r="D60" t="s">
         <v>203</v>
       </c>
-      <c r="C35" t="s">
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>71</v>
+      </c>
+      <c r="B61" t="s">
+        <v>143</v>
+      </c>
+      <c r="C61" t="s">
         <v>204</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D61" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
-      <c r="A36" t="s">
-        <v>65</v>
-      </c>
-      <c r="B36" t="s">
-        <v>206</v>
-      </c>
-      <c r="C36" t="s">
-        <v>207</v>
-      </c>
-      <c r="D36" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" t="s">
-        <v>65</v>
-      </c>
-      <c r="B37" t="s">
-        <v>208</v>
-      </c>
-      <c r="C37" t="s">
-        <v>209</v>
-      </c>
-      <c r="D37" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" t="s">
-        <v>65</v>
-      </c>
-      <c r="B38" t="s">
-        <v>211</v>
-      </c>
-      <c r="C38" t="s">
-        <v>212</v>
-      </c>
-      <c r="D38" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" t="s">
-        <v>65</v>
-      </c>
-      <c r="B39" t="s">
-        <v>214</v>
-      </c>
-      <c r="C39" t="s">
-        <v>215</v>
-      </c>
-      <c r="D39" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="A41" t="s">
-        <v>85</v>
-      </c>
-      <c r="B41" t="s">
-        <v>217</v>
-      </c>
-      <c r="C41" t="s">
-        <v>218</v>
-      </c>
-      <c r="D41" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="A42" t="s">
-        <v>85</v>
-      </c>
-      <c r="B42" t="s">
-        <v>219</v>
-      </c>
-      <c r="C42" t="s">
-        <v>220</v>
-      </c>
-      <c r="D42" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="A43" t="s">
-        <v>85</v>
-      </c>
-      <c r="B43" t="s">
-        <v>222</v>
-      </c>
-      <c r="C43" t="s">
-        <v>223</v>
-      </c>
-      <c r="D43" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" t="s">
-        <v>94</v>
-      </c>
-      <c r="B45" t="s">
-        <v>225</v>
-      </c>
-      <c r="C45" t="s">
-        <v>226</v>
-      </c>
-      <c r="D45" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="A46" t="s">
-        <v>94</v>
-      </c>
-      <c r="B46" t="s">
-        <v>228</v>
-      </c>
-      <c r="C46" t="s">
-        <v>229</v>
-      </c>
-      <c r="D46" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="A47" t="s">
-        <v>94</v>
-      </c>
-      <c r="B47" t="s">
-        <v>184</v>
-      </c>
-      <c r="C47" t="s">
-        <v>231</v>
-      </c>
-      <c r="D47" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
-      <c r="A49" t="s">
-        <v>99</v>
-      </c>
-      <c r="B49" t="s">
-        <v>233</v>
-      </c>
-      <c r="C49" t="s">
-        <v>234</v>
-      </c>
-      <c r="D49" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4">
-      <c r="A50" t="s">
-        <v>99</v>
-      </c>
-      <c r="B50" t="s">
-        <v>236</v>
-      </c>
-      <c r="C50" t="s">
-        <v>237</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4">
-      <c r="A51" t="s">
-        <v>99</v>
-      </c>
-      <c r="B51" t="s">
-        <v>184</v>
-      </c>
-      <c r="C51" t="s">
-        <v>239</v>
-      </c>
-      <c r="D51" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
-      <c r="A52" t="s">
-        <v>99</v>
-      </c>
-      <c r="B52" t="s">
-        <v>187</v>
-      </c>
-      <c r="C52" t="s">
-        <v>188</v>
-      </c>
-      <c r="D52" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4">
-      <c r="A54" t="s">
-        <v>112</v>
-      </c>
-      <c r="B54" t="s">
-        <v>241</v>
-      </c>
-      <c r="C54" t="s">
-        <v>242</v>
-      </c>
-      <c r="D54" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4">
-      <c r="A55" t="s">
-        <v>112</v>
-      </c>
-      <c r="B55" t="s">
-        <v>244</v>
-      </c>
-      <c r="C55" t="s">
-        <v>245</v>
-      </c>
-      <c r="D55" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4">
-      <c r="A56" t="s">
-        <v>112</v>
-      </c>
-      <c r="B56" t="s">
-        <v>184</v>
-      </c>
-      <c r="C56" t="s">
-        <v>247</v>
-      </c>
-      <c r="D56" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4">
-      <c r="A57" t="s">
-        <v>112</v>
-      </c>
-      <c r="B57" t="s">
-        <v>187</v>
-      </c>
-      <c r="C57" t="s">
-        <v>188</v>
-      </c>
-      <c r="D57" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4">
-      <c r="A58" t="s">
-        <v>112</v>
-      </c>
-      <c r="B58" t="s">
-        <v>211</v>
-      </c>
-      <c r="C58" t="s">
-        <v>212</v>
-      </c>
-      <c r="D58" t="s">
-        <v>213</v>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>71</v>
+      </c>
+      <c r="B62" t="s">
+        <v>146</v>
+      </c>
+      <c r="C62" t="s">
+        <v>147</v>
+      </c>
+      <c r="D62" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>71</v>
+      </c>
+      <c r="B63" t="s">
+        <v>170</v>
+      </c>
+      <c r="C63" t="s">
+        <v>171</v>
+      </c>
+      <c r="D63" t="s">
+        <v>172</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2873,10 +3050,10 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="21.5" customWidth="1"/>
     <col min="2" max="2" width="23.33203125" customWidth="1"/>
@@ -2892,99 +3069,99 @@
     <col min="12" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="21" customHeight="1">
+    <row r="1" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>249</v>
+        <v>206</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>250</v>
+        <v>207</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>251</v>
+        <v>208</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>252</v>
+        <v>209</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>253</v>
+        <v>210</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>254</v>
+        <v>211</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>255</v>
+        <v>212</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>256</v>
+        <v>213</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>257</v>
+        <v>214</v>
       </c>
       <c r="J1" t="s">
-        <v>258</v>
+        <v>215</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="26" customHeight="1">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="26" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>260</v>
+        <v>217</v>
       </c>
       <c r="B2" t="s">
-        <v>261</v>
+        <v>218</v>
       </c>
       <c r="C2" t="s">
-        <v>262</v>
+        <v>219</v>
       </c>
       <c r="D2" t="s">
-        <v>262</v>
+        <v>219</v>
       </c>
       <c r="E2" t="s">
-        <v>263</v>
+        <v>220</v>
       </c>
       <c r="F2" t="s">
-        <v>264</v>
+        <v>221</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>265</v>
+        <v>222</v>
       </c>
       <c r="J2" t="s">
-        <v>266</v>
+        <v>223</v>
       </c>
       <c r="K2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="45.75" customHeight="1">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="45.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:11" ht="64.75" customHeight="1">
+    <row r="4" spans="1:11" ht="64.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:11" ht="62" customHeight="1">
+    <row r="5" spans="1:11" ht="62" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>267</v>
+        <v>224</v>
       </c>
       <c r="H5" t="s">
-        <v>268</v>
+        <v>225</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>269</v>
+        <v>226</v>
       </c>
       <c r="J5" t="s">
-        <v>266</v>
+        <v>223</v>
       </c>
       <c r="K5" t="s">
-        <v>266</v>
+        <v>223</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3001,7 +3178,7 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="10.5" customWidth="1"/>
@@ -3009,12 +3186,12 @@
     <col min="4" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>270</v>
+        <v>227</v>
       </c>
       <c r="B1" t="s">
-        <v>271</v>
+        <v>228</v>
       </c>
       <c r="C1" t="s">
         <v>5</v>
@@ -3023,89 +3200,89 @@
         <v>6</v>
       </c>
       <c r="E1" t="s">
-        <v>272</v>
+        <v>229</v>
       </c>
       <c r="F1" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>274</v>
+        <v>231</v>
       </c>
       <c r="B2" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>276</v>
+        <v>233</v>
       </c>
       <c r="C4" t="s">
-        <v>277</v>
+        <v>234</v>
       </c>
       <c r="D4" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>279</v>
+        <v>236</v>
       </c>
       <c r="B5" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="30">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="31" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
-        <v>280</v>
+        <v>237</v>
       </c>
       <c r="B6" s="2" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>281</v>
+        <v>238</v>
       </c>
       <c r="B7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
-        <v>282</v>
+        <v>239</v>
       </c>
       <c r="B8" s="7">
         <v>20170807</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>283</v>
+        <v>240</v>
       </c>
       <c r="E9" t="s">
-        <v>284</v>
+        <v>241</v>
       </c>
       <c r="F9" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>286</v>
+        <v>243</v>
       </c>
       <c r="E10" t="s">
-        <v>287</v>
+        <v>244</v>
       </c>
       <c r="F10" t="s">
-        <v>288</v>
+        <v>245</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3122,227 +3299,227 @@
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="10.5" customWidth="1"/>
     <col min="3" max="3" width="31.1640625" customWidth="1"/>
     <col min="4" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>289</v>
+        <v>246</v>
       </c>
       <c r="B1" t="s">
-        <v>290</v>
+        <v>247</v>
       </c>
       <c r="C1" t="s">
-        <v>291</v>
+        <v>248</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>292</v>
+        <v>249</v>
       </c>
       <c r="B2" t="s">
-        <v>293</v>
+        <v>250</v>
       </c>
       <c r="C2" t="s">
-        <v>294</v>
+        <v>251</v>
       </c>
       <c r="D2" t="s">
-        <v>295</v>
+        <v>252</v>
       </c>
       <c r="E2" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>292</v>
+        <v>249</v>
       </c>
       <c r="B3" t="s">
-        <v>293</v>
+        <v>250</v>
       </c>
       <c r="C3" t="s">
-        <v>297</v>
+        <v>254</v>
       </c>
       <c r="D3" t="s">
-        <v>295</v>
+        <v>252</v>
       </c>
       <c r="E3" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>292</v>
+        <v>249</v>
       </c>
       <c r="B4" t="s">
-        <v>293</v>
+        <v>250</v>
       </c>
       <c r="C4" t="s">
-        <v>298</v>
+        <v>255</v>
       </c>
       <c r="D4" t="s">
-        <v>295</v>
+        <v>252</v>
       </c>
       <c r="E4" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>292</v>
+        <v>249</v>
       </c>
       <c r="B5" t="s">
-        <v>293</v>
+        <v>250</v>
       </c>
       <c r="C5" t="s">
-        <v>299</v>
+        <v>256</v>
       </c>
       <c r="D5" t="s">
-        <v>295</v>
+        <v>252</v>
       </c>
       <c r="E5" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>300</v>
+        <v>257</v>
       </c>
       <c r="B6" t="s">
-        <v>293</v>
+        <v>250</v>
       </c>
       <c r="C6" t="s">
-        <v>301</v>
+        <v>258</v>
       </c>
       <c r="D6" t="s">
-        <v>295</v>
+        <v>252</v>
       </c>
       <c r="E6" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>300</v>
+        <v>257</v>
       </c>
       <c r="B7" t="s">
-        <v>293</v>
+        <v>250</v>
       </c>
       <c r="C7" t="s">
-        <v>302</v>
+        <v>259</v>
       </c>
       <c r="D7" t="s">
-        <v>295</v>
+        <v>252</v>
       </c>
       <c r="E7" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>300</v>
+        <v>257</v>
       </c>
       <c r="B8" t="s">
-        <v>293</v>
+        <v>250</v>
       </c>
       <c r="C8" t="s">
-        <v>304</v>
+        <v>261</v>
       </c>
       <c r="D8" t="s">
-        <v>295</v>
+        <v>252</v>
       </c>
       <c r="E8" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>292</v>
+        <v>249</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>306</v>
+        <v>263</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>307</v>
+        <v>264</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>308</v>
+        <v>265</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
-        <v>292</v>
+        <v>249</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>306</v>
+        <v>263</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>310</v>
+        <v>267</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>295</v>
+        <v>252</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="8"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
-        <v>312</v>
+        <v>269</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>293</v>
+        <v>250</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>313</v>
+        <v>270</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>295</v>
+        <v>252</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
-        <v>315</v>
+        <v>272</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>293</v>
+        <v>250</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>316</v>
+        <v>273</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>295</v>
+        <v>252</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>317</v>
+        <v>274</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3359,12 +3536,12 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1025" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -3372,25 +3549,25 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>318</v>
+        <v>275</v>
       </c>
       <c r="B2" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>319</v>
+        <v>276</v>
       </c>
       <c r="B3" t="s">
-        <v>295</v>
+        <v>252</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"DejaVu Serif,Book"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"DejaVu Serif,Book"Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Move health facility summary information to a different screen
</commit_message>
<xml_diff>
--- a/app/config/tables/health_facility/forms/health_facility/health_facility.xlsx
+++ b/app/config/tables/health_facility/forms/health_facility/health_facility.xlsx
@@ -19,7 +19,7 @@
     <sheet name="properties" sheetId="5" r:id="rId5"/>
     <sheet name="model" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="162913" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="344">
   <si>
     <t>clause</t>
   </si>
@@ -1612,10 +1612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K44"/>
+  <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C22" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1968,119 +1968,149 @@
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
+      <c r="C23" t="s">
+        <v>44</v>
+      </c>
+      <c r="E23" t="s">
+        <v>61</v>
+      </c>
+      <c r="F23" t="s">
+        <v>62</v>
+      </c>
+      <c r="G23" t="s">
+        <v>63</v>
+      </c>
+      <c r="H23" t="s">
+        <v>64</v>
+      </c>
+      <c r="I23" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C24" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24" t="s">
+        <v>316</v>
+      </c>
+      <c r="E24" t="s">
+        <v>314</v>
+      </c>
+      <c r="F24" t="s">
+        <v>315</v>
+      </c>
+      <c r="G24" t="s">
+        <v>66</v>
+      </c>
+      <c r="H24" t="s">
+        <v>67</v>
+      </c>
+      <c r="I24" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="C25" t="s">
-        <v>44</v>
-      </c>
-      <c r="E25" t="s">
-        <v>61</v>
-      </c>
-      <c r="F25" t="s">
-        <v>62</v>
-      </c>
-      <c r="G25" t="s">
-        <v>63</v>
-      </c>
-      <c r="H25" t="s">
-        <v>64</v>
-      </c>
-      <c r="I25" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="C26" t="s">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C27" t="s">
+        <v>43</v>
+      </c>
+      <c r="E27" t="s">
+        <v>68</v>
+      </c>
+      <c r="F27" t="s">
+        <v>69</v>
+      </c>
+      <c r="G27" t="s">
+        <v>70</v>
+      </c>
+      <c r="H27" t="s">
+        <v>320</v>
+      </c>
+      <c r="I27" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C28" t="s">
         <v>32</v>
       </c>
-      <c r="D26" t="s">
-        <v>316</v>
-      </c>
-      <c r="E26" t="s">
-        <v>314</v>
-      </c>
-      <c r="F26" t="s">
-        <v>315</v>
-      </c>
-      <c r="G26" t="s">
-        <v>66</v>
-      </c>
-      <c r="H26" t="s">
-        <v>67</v>
-      </c>
-      <c r="I26" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
+      <c r="D28" t="s">
+        <v>71</v>
+      </c>
+      <c r="E28" t="s">
+        <v>72</v>
+      </c>
+      <c r="F28" t="s">
+        <v>73</v>
+      </c>
+      <c r="G28" t="s">
+        <v>74</v>
+      </c>
+      <c r="H28" t="s">
+        <v>75</v>
+      </c>
+      <c r="I28" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="C29" t="s">
-        <v>43</v>
-      </c>
-      <c r="E29" t="s">
-        <v>68</v>
-      </c>
-      <c r="F29" t="s">
-        <v>69</v>
-      </c>
-      <c r="G29" t="s">
-        <v>70</v>
-      </c>
-      <c r="H29" t="s">
-        <v>320</v>
-      </c>
-      <c r="I29" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="C30" t="s">
-        <v>32</v>
-      </c>
-      <c r="D30" t="s">
-        <v>71</v>
-      </c>
-      <c r="E30" t="s">
-        <v>72</v>
-      </c>
-      <c r="F30" t="s">
-        <v>73</v>
-      </c>
-      <c r="G30" t="s">
-        <v>74</v>
-      </c>
-      <c r="H30" t="s">
-        <v>75</v>
-      </c>
-      <c r="I30" t="s">
-        <v>323</v>
-      </c>
-    </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>21</v>
+      <c r="C31" t="s">
+        <v>12</v>
+      </c>
+      <c r="E31" t="s">
+        <v>76</v>
+      </c>
+      <c r="F31" t="s">
+        <v>77</v>
+      </c>
+      <c r="G31" t="s">
+        <v>78</v>
+      </c>
+      <c r="H31" t="s">
+        <v>79</v>
+      </c>
+      <c r="I31" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>11</v>
+      <c r="C32" t="s">
+        <v>12</v>
+      </c>
+      <c r="E32" t="s">
+        <v>281</v>
+      </c>
+      <c r="F32" t="s">
+        <v>282</v>
+      </c>
+      <c r="G32" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="H32" t="s">
+        <v>294</v>
+      </c>
+      <c r="I32" s="10" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.35">
@@ -2088,165 +2118,125 @@
         <v>12</v>
       </c>
       <c r="E33" t="s">
-        <v>76</v>
+        <v>283</v>
       </c>
       <c r="F33" t="s">
-        <v>77</v>
-      </c>
-      <c r="G33" t="s">
-        <v>78</v>
+        <v>284</v>
+      </c>
+      <c r="G33" s="11" t="s">
+        <v>296</v>
       </c>
       <c r="H33" t="s">
-        <v>79</v>
-      </c>
-      <c r="I33" t="s">
-        <v>324</v>
+        <v>284</v>
+      </c>
+      <c r="I33" s="11" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="C34" t="s">
-        <v>12</v>
-      </c>
-      <c r="E34" t="s">
-        <v>281</v>
-      </c>
-      <c r="F34" t="s">
-        <v>282</v>
-      </c>
-      <c r="G34" s="10" t="s">
-        <v>293</v>
-      </c>
-      <c r="H34" t="s">
-        <v>294</v>
-      </c>
-      <c r="I34" s="10" t="s">
-        <v>295</v>
+      <c r="A34" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="C35" t="s">
-        <v>12</v>
-      </c>
-      <c r="E35" t="s">
-        <v>283</v>
-      </c>
-      <c r="F35" t="s">
-        <v>284</v>
-      </c>
-      <c r="G35" s="11" t="s">
-        <v>296</v>
-      </c>
-      <c r="H35" t="s">
-        <v>284</v>
-      </c>
-      <c r="I35" s="11" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
+      <c r="A35" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C36" t="s">
+        <v>43</v>
+      </c>
+      <c r="E36" t="s">
+        <v>289</v>
+      </c>
+      <c r="F36" t="s">
+        <v>285</v>
+      </c>
+      <c r="G36" s="11" t="s">
+        <v>302</v>
+      </c>
+      <c r="H36" t="s">
+        <v>298</v>
+      </c>
+      <c r="I36" s="11" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C37" t="s">
+        <v>43</v>
+      </c>
+      <c r="E37" t="s">
+        <v>290</v>
+      </c>
+      <c r="F37" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="G37" s="12" t="s">
+        <v>303</v>
+      </c>
+      <c r="H37" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="I37" s="12" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A38" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
+      <c r="F38" s="9"/>
+    </row>
+    <row r="39" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A39" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C38" t="s">
+      <c r="F39" s="9"/>
+    </row>
+    <row r="40" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C40" t="s">
         <v>43</v>
       </c>
-      <c r="E38" t="s">
-        <v>289</v>
-      </c>
-      <c r="F38" t="s">
-        <v>285</v>
-      </c>
-      <c r="G38" s="11" t="s">
-        <v>302</v>
-      </c>
-      <c r="H38" t="s">
-        <v>298</v>
-      </c>
-      <c r="I38" s="11" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C39" t="s">
+      <c r="E40" t="s">
+        <v>291</v>
+      </c>
+      <c r="F40" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="G40" s="12" t="s">
+        <v>306</v>
+      </c>
+      <c r="H40" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="I40" s="12" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C41" t="s">
         <v>43</v>
       </c>
-      <c r="E39" t="s">
-        <v>290</v>
-      </c>
-      <c r="F39" s="9" t="s">
-        <v>286</v>
-      </c>
-      <c r="G39" s="12" t="s">
-        <v>303</v>
-      </c>
-      <c r="H39" s="9" t="s">
-        <v>299</v>
-      </c>
-      <c r="I39" s="12" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A40" t="s">
-        <v>21</v>
-      </c>
-      <c r="F40" s="9"/>
-    </row>
-    <row r="41" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A41" t="s">
-        <v>11</v>
-      </c>
-      <c r="F41" s="9"/>
-    </row>
-    <row r="42" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C42" t="s">
-        <v>43</v>
-      </c>
-      <c r="E42" t="s">
-        <v>291</v>
-      </c>
-      <c r="F42" s="9" t="s">
-        <v>287</v>
-      </c>
-      <c r="G42" s="12" t="s">
-        <v>306</v>
-      </c>
-      <c r="H42" s="9" t="s">
-        <v>300</v>
-      </c>
-      <c r="I42" s="12" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C43" t="s">
-        <v>43</v>
-      </c>
-      <c r="E43" t="s">
+      <c r="E41" t="s">
         <v>292</v>
       </c>
-      <c r="F43" s="9" t="s">
+      <c r="F41" s="9" t="s">
         <v>288</v>
       </c>
-      <c r="G43" s="12" t="s">
+      <c r="G41" s="12" t="s">
         <v>308</v>
       </c>
-      <c r="H43" s="9" t="s">
+      <c r="H41" s="9" t="s">
         <v>301</v>
       </c>
-      <c r="I43" s="12" t="s">
+      <c r="I41" s="12" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>